<commit_message>
Doc: updated Supplier Test Cases according to review comments
</commit_message>
<xml_diff>
--- a/Test/Test-cases.xlsx
+++ b/Test/Test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC44F2B0-058C-491E-ADA6-16B25ACEF975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DAB00C-E5CF-4A43-9A88-6206B9A716E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="234">
   <si>
     <t>Test case ID</t>
   </si>
@@ -1101,6 +1101,11 @@
   <si>
     <t>1.Search for the product using its Product ID                                                                                                       2. Click "Delete" on product
 3. Confirm deletion</t>
+  </si>
+  <si>
+    <t>1. Type "valid-email" in email field
+2. Fill other fields with valid data
+3. Click "Register"</t>
   </si>
 </sst>
 </file>
@@ -1265,36 +1270,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1306,21 +1303,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1542,8 +1547,8 @@
   </sheetPr>
   <dimension ref="A1:S970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41:L42"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="79" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1563,12 +1568,12 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="24" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="15" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="25"/>
@@ -1585,7 +1590,7 @@
       </c>
       <c r="N1" s="28"/>
       <c r="O1" s="29"/>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="Q1" s="26"/>
@@ -1601,8 +1606,8 @@
       <c r="B2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="9" t="s">
         <v>57</v>
       </c>
@@ -1631,8 +1636,8 @@
       <c r="B3" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="31"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
       <c r="E3" s="12" t="s">
         <v>62</v>
       </c>
@@ -1645,11 +1650,11 @@
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="17"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="37"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="11"/>
       <c r="R3" s="3"/>
@@ -1661,8 +1666,8 @@
       <c r="B4" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
       <c r="E4" s="12" t="s">
         <v>62</v>
       </c>
@@ -1678,8 +1683,8 @@
       <c r="M4" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N4" s="13"/>
-      <c r="O4" s="14"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="3"/>
@@ -1691,8 +1696,8 @@
       <c r="B5" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="31"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="12" t="s">
         <v>69</v>
       </c>
@@ -1708,8 +1713,8 @@
       <c r="M5" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N5" s="13"/>
-      <c r="O5" s="14"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="11"/>
       <c r="R5" s="3"/>
@@ -1721,8 +1726,8 @@
       <c r="B6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="12" t="s">
         <v>62</v>
       </c>
@@ -1751,8 +1756,8 @@
       <c r="B7" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="12" t="s">
         <v>76</v>
       </c>
@@ -1760,7 +1765,7 @@
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="9" t="s">
-        <v>73</v>
+        <v>233</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -1781,8 +1786,8 @@
       <c r="B8" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="12" t="s">
         <v>62</v>
       </c>
@@ -1798,8 +1803,8 @@
       <c r="M8" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="14"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="19"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="11"/>
       <c r="R8" s="3"/>
@@ -1811,8 +1816,8 @@
       <c r="B9" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="12" t="s">
         <v>62</v>
       </c>
@@ -1841,8 +1846,8 @@
       <c r="B10" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="12" t="s">
         <v>62</v>
       </c>
@@ -1858,8 +1863,8 @@
       <c r="M10" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="N10" s="13"/>
-      <c r="O10" s="14"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="19"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="3"/>
@@ -1871,8 +1876,8 @@
       <c r="B11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="12" t="s">
         <v>62</v>
       </c>
@@ -1888,8 +1893,8 @@
       <c r="M11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N11" s="13"/>
-      <c r="O11" s="14"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="19"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="11"/>
       <c r="R11" s="3"/>
@@ -1901,8 +1906,8 @@
       <c r="B12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="12" t="s">
         <v>62</v>
       </c>
@@ -1918,8 +1923,8 @@
       <c r="M12" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N12" s="13"/>
-      <c r="O12" s="14"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="19"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="11"/>
       <c r="R12" s="3"/>
@@ -1931,8 +1936,8 @@
       <c r="B13" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="12" t="s">
         <v>62</v>
       </c>
@@ -1961,8 +1966,8 @@
       <c r="B14" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="12" t="s">
         <v>62</v>
       </c>
@@ -1991,8 +1996,8 @@
       <c r="B15" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="12" t="s">
         <v>102</v>
       </c>
@@ -2021,8 +2026,8 @@
       <c r="B16" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="12" t="s">
         <v>62</v>
       </c>
@@ -2051,8 +2056,8 @@
       <c r="B17" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="12" t="s">
         <v>62</v>
       </c>
@@ -2081,8 +2086,8 @@
       <c r="B18" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="12" t="s">
         <v>62</v>
       </c>
@@ -2106,22 +2111,22 @@
     </row>
     <row r="19" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="20"/>
+      <c r="Q19" s="24"/>
       <c r="R19" s="6"/>
       <c r="S19" s="8"/>
     </row>
@@ -2132,8 +2137,8 @@
       <c r="B20" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="9" t="s">
         <v>8</v>
       </c>
@@ -2162,8 +2167,8 @@
       <c r="B21" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="9" t="s">
         <v>8</v>
       </c>
@@ -2192,8 +2197,8 @@
       <c r="B22" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="9" t="s">
         <v>8</v>
       </c>
@@ -2222,8 +2227,8 @@
       <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
       <c r="E23" s="9" t="s">
         <v>8</v>
       </c>
@@ -2252,8 +2257,8 @@
       <c r="B24" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="9" t="s">
         <v>8</v>
       </c>
@@ -2269,8 +2274,8 @@
       <c r="M24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N24" s="32"/>
-      <c r="O24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="34"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="11"/>
       <c r="R24" s="3"/>
@@ -2282,8 +2287,8 @@
       <c r="B25" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="9" t="s">
         <v>8</v>
       </c>
@@ -2299,8 +2304,8 @@
       <c r="M25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="N25" s="32"/>
-      <c r="O25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="34"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="11"/>
       <c r="R25" s="3"/>
@@ -2312,8 +2317,8 @@
       <c r="B26" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="9" t="s">
         <v>8</v>
       </c>
@@ -2342,8 +2347,8 @@
       <c r="B27" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
       <c r="E27" s="9" t="s">
         <v>8</v>
       </c>
@@ -2372,8 +2377,8 @@
       <c r="B28" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="9" t="s">
         <v>8</v>
       </c>
@@ -2402,8 +2407,8 @@
       <c r="B29" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="9" t="s">
         <v>8</v>
       </c>
@@ -2432,8 +2437,8 @@
       <c r="B30" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="31"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="9" t="s">
         <v>8</v>
       </c>
@@ -2462,8 +2467,8 @@
       <c r="B31" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="9" t="s">
         <v>8</v>
       </c>
@@ -2492,8 +2497,8 @@
       <c r="B32" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
       <c r="E32" s="9" t="s">
         <v>8</v>
       </c>
@@ -2522,8 +2527,8 @@
       <c r="B33" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
       <c r="E33" s="9" t="s">
         <v>8</v>
       </c>
@@ -2547,22 +2552,22 @@
     </row>
     <row r="34" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="19"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="24"/>
       <c r="R34" s="6"/>
       <c r="S34" s="8"/>
     </row>
@@ -2573,8 +2578,8 @@
       <c r="B35" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
       <c r="E35" s="9" t="s">
         <v>116</v>
       </c>
@@ -2603,8 +2608,8 @@
       <c r="B36" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
       <c r="E36" s="12" t="s">
         <v>121</v>
       </c>
@@ -2633,8 +2638,8 @@
       <c r="B37" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
       <c r="E37" s="12" t="s">
         <v>121</v>
       </c>
@@ -2650,8 +2655,8 @@
       <c r="M37" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="N37" s="13"/>
-      <c r="O37" s="14"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="19"/>
       <c r="P37" s="12"/>
       <c r="Q37" s="11"/>
       <c r="R37" s="3"/>
@@ -2663,8 +2668,8 @@
       <c r="B38" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
       <c r="E38" s="12" t="s">
         <v>121</v>
       </c>
@@ -2680,8 +2685,8 @@
       <c r="M38" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="N38" s="13"/>
-      <c r="O38" s="14"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="19"/>
       <c r="P38" s="12"/>
       <c r="Q38" s="11"/>
       <c r="R38" s="3"/>
@@ -2693,8 +2698,8 @@
       <c r="B39" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
       <c r="E39" s="12" t="s">
         <v>121</v>
       </c>
@@ -2710,8 +2715,8 @@
       <c r="M39" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="N39" s="13"/>
-      <c r="O39" s="14"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="19"/>
       <c r="P39" s="12"/>
       <c r="Q39" s="11"/>
       <c r="R39" s="3"/>
@@ -2723,8 +2728,8 @@
       <c r="B40" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
       <c r="E40" s="12" t="s">
         <v>121</v>
       </c>
@@ -2737,11 +2742,11 @@
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
       <c r="L40" s="11"/>
-      <c r="M40" s="21" t="s">
+      <c r="M40" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="N40" s="22"/>
-      <c r="O40" s="23"/>
+      <c r="N40" s="31"/>
+      <c r="O40" s="32"/>
       <c r="P40" s="12"/>
       <c r="Q40" s="11"/>
       <c r="R40" s="3"/>
@@ -2753,8 +2758,8 @@
       <c r="B41" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
       <c r="E41" s="12" t="s">
         <v>138</v>
       </c>
@@ -2783,8 +2788,8 @@
       <c r="B42" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
       <c r="E42" s="12" t="s">
         <v>138</v>
       </c>
@@ -2808,22 +2813,22 @@
     </row>
     <row r="43" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="19"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="19"/>
-      <c r="P43" s="18"/>
-      <c r="Q43" s="19"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="24"/>
       <c r="R43" s="6"/>
       <c r="S43" s="8"/>
     </row>
@@ -2834,8 +2839,8 @@
       <c r="B44" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
       <c r="E44" s="12" t="s">
         <v>221</v>
       </c>
@@ -2851,8 +2856,8 @@
       <c r="M44" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="N44" s="13"/>
-      <c r="O44" s="14"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="19"/>
       <c r="P44" s="12"/>
       <c r="Q44" s="11"/>
       <c r="R44" s="3"/>
@@ -2864,8 +2869,8 @@
       <c r="B45" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
       <c r="E45" s="12" t="s">
         <v>147</v>
       </c>
@@ -2881,8 +2886,8 @@
       <c r="M45" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="N45" s="13"/>
-      <c r="O45" s="14"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="19"/>
       <c r="P45" s="12"/>
       <c r="Q45" s="11"/>
       <c r="R45" s="3"/>
@@ -2894,8 +2899,8 @@
       <c r="B46" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
       <c r="E46" s="12" t="s">
         <v>148</v>
       </c>
@@ -2905,14 +2910,14 @@
       <c r="I46" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="J46" s="13"/>
-      <c r="K46" s="13"/>
-      <c r="L46" s="14"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="19"/>
       <c r="M46" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="N46" s="13"/>
-      <c r="O46" s="14"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="19"/>
       <c r="P46" s="12"/>
       <c r="Q46" s="11"/>
       <c r="R46" s="3"/>
@@ -2924,8 +2929,8 @@
       <c r="B47" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
       <c r="E47" s="12" t="s">
         <v>177</v>
       </c>
@@ -2935,14 +2940,14 @@
       <c r="I47" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="14"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="19"/>
       <c r="M47" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="N47" s="13"/>
-      <c r="O47" s="14"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="19"/>
       <c r="P47" s="12"/>
       <c r="Q47" s="11"/>
       <c r="R47" s="3"/>
@@ -2954,8 +2959,8 @@
       <c r="B48" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="31"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
       <c r="E48" s="12" t="s">
         <v>176</v>
       </c>
@@ -2965,14 +2970,14 @@
       <c r="I48" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="J48" s="13"/>
-      <c r="K48" s="13"/>
-      <c r="L48" s="14"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="19"/>
       <c r="M48" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="N48" s="13"/>
-      <c r="O48" s="14"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="19"/>
       <c r="P48" s="12"/>
       <c r="Q48" s="11"/>
       <c r="R48" s="3"/>
@@ -2984,8 +2989,8 @@
       <c r="B49" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C49" s="30"/>
-      <c r="D49" s="31"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
       <c r="E49" s="12" t="s">
         <v>175</v>
       </c>
@@ -2995,14 +3000,14 @@
       <c r="I49" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="14"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="19"/>
       <c r="M49" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="N49" s="13"/>
-      <c r="O49" s="14"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="19"/>
       <c r="P49" s="12"/>
       <c r="Q49" s="11"/>
       <c r="R49" s="3"/>
@@ -3014,8 +3019,8 @@
       <c r="B50" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="31"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
       <c r="E50" s="12" t="s">
         <v>174</v>
       </c>
@@ -3025,14 +3030,14 @@
       <c r="I50" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="14"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="19"/>
       <c r="M50" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="N50" s="13"/>
-      <c r="O50" s="14"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="19"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="11"/>
       <c r="R50" s="3"/>
@@ -3044,8 +3049,8 @@
       <c r="B51" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="31"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
       <c r="E51" s="12" t="s">
         <v>189</v>
       </c>
@@ -3061,8 +3066,8 @@
       <c r="M51" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="N51" s="13"/>
-      <c r="O51" s="14"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="19"/>
       <c r="P51" s="12"/>
       <c r="Q51" s="11"/>
       <c r="R51" s="3"/>
@@ -3074,8 +3079,8 @@
       <c r="B52" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="31"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
       <c r="E52" s="12" t="s">
         <v>190</v>
       </c>
@@ -3091,8 +3096,8 @@
       <c r="M52" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="N52" s="13"/>
-      <c r="O52" s="14"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="19"/>
       <c r="P52" s="12"/>
       <c r="Q52" s="11"/>
       <c r="R52" s="3"/>
@@ -3104,14 +3109,14 @@
       <c r="B53" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C53" s="30"/>
-      <c r="D53" s="31"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
       <c r="E53" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="14"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="19"/>
       <c r="I53" s="9" t="s">
         <v>217</v>
       </c>
@@ -3134,25 +3139,25 @@
       <c r="B54" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="31"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
       <c r="E54" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="14"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19"/>
       <c r="I54" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="J54" s="13"/>
-      <c r="K54" s="13"/>
-      <c r="L54" s="14"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="19"/>
       <c r="M54" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="N54" s="13"/>
-      <c r="O54" s="14"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="19"/>
       <c r="P54" s="12"/>
       <c r="Q54" s="11"/>
       <c r="R54" s="3"/>
@@ -3164,25 +3169,25 @@
       <c r="B55" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C55" s="30"/>
-      <c r="D55" s="31"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="14"/>
       <c r="E55" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="14"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="19"/>
       <c r="I55" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="J55" s="13"/>
-      <c r="K55" s="13"/>
-      <c r="L55" s="14"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="19"/>
       <c r="M55" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="N55" s="13"/>
-      <c r="O55" s="14"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="19"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="11"/>
       <c r="R55" s="3"/>
@@ -3194,25 +3199,25 @@
       <c r="B56" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C56" s="30"/>
-      <c r="D56" s="31"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="14"/>
       <c r="E56" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="14"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="19"/>
       <c r="I56" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="J56" s="13"/>
-      <c r="K56" s="13"/>
-      <c r="L56" s="14"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="19"/>
       <c r="M56" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="N56" s="13"/>
-      <c r="O56" s="14"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="19"/>
       <c r="P56" s="12"/>
       <c r="Q56" s="11"/>
       <c r="R56" s="3"/>
@@ -3224,14 +3229,14 @@
       <c r="B57" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C57" s="30"/>
-      <c r="D57" s="31"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="14"/>
       <c r="E57" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="14"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="19"/>
       <c r="I57" s="12" t="s">
         <v>188</v>
       </c>
@@ -3241,8 +3246,8 @@
       <c r="M57" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="N57" s="13"/>
-      <c r="O57" s="14"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="19"/>
       <c r="P57" s="12"/>
       <c r="Q57" s="11"/>
       <c r="R57" s="3"/>
@@ -3254,8 +3259,8 @@
       <c r="B58" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C58" s="30"/>
-      <c r="D58" s="31"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="14"/>
       <c r="E58" s="9" t="s">
         <v>204</v>
       </c>
@@ -3284,8 +3289,8 @@
       <c r="B59" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C59" s="30"/>
-      <c r="D59" s="31"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="14"/>
       <c r="E59" s="12" t="s">
         <v>205</v>
       </c>
@@ -3295,14 +3300,14 @@
       <c r="I59" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="J59" s="13"/>
-      <c r="K59" s="13"/>
-      <c r="L59" s="14"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="19"/>
       <c r="M59" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="N59" s="13"/>
-      <c r="O59" s="14"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="19"/>
       <c r="P59" s="12"/>
       <c r="Q59" s="11"/>
       <c r="R59" s="3"/>
@@ -3314,8 +3319,8 @@
       <c r="B60" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C60" s="30"/>
-      <c r="D60" s="31"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="14"/>
       <c r="E60" s="12" t="s">
         <v>210</v>
       </c>
@@ -3325,14 +3330,14 @@
       <c r="I60" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="J60" s="13"/>
-      <c r="K60" s="13"/>
-      <c r="L60" s="14"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="19"/>
       <c r="M60" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="N60" s="13"/>
-      <c r="O60" s="14"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="19"/>
       <c r="P60" s="12"/>
       <c r="Q60" s="11"/>
       <c r="R60" s="3"/>
@@ -3344,25 +3349,25 @@
       <c r="B61" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C61" s="30"/>
-      <c r="D61" s="31"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="14"/>
       <c r="E61" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="14"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="19"/>
       <c r="I61" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="J61" s="13"/>
-      <c r="K61" s="13"/>
-      <c r="L61" s="14"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="19"/>
       <c r="M61" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="N61" s="13"/>
-      <c r="O61" s="14"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="19"/>
       <c r="P61" s="12"/>
       <c r="Q61" s="11"/>
       <c r="R61" s="3"/>
@@ -3370,8 +3375,8 @@
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="12"/>
-      <c r="C62" s="30"/>
-      <c r="D62" s="31"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
       <c r="E62" s="12"/>
       <c r="F62" s="10"/>
       <c r="G62" s="10"/>
@@ -3390,8 +3395,8 @@
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="12"/>
-      <c r="C63" s="30"/>
-      <c r="D63" s="31"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="14"/>
       <c r="E63" s="12"/>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
@@ -3410,8 +3415,8 @@
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="12"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="31"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="14"/>
       <c r="E64" s="12"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
@@ -3430,8 +3435,8 @@
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="12"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="31"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="14"/>
       <c r="E65" s="12"/>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
@@ -3450,8 +3455,8 @@
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="30"/>
-      <c r="D66" s="31"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
       <c r="E66" s="12"/>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
@@ -3470,8 +3475,8 @@
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="12"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="31"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
       <c r="E67" s="12"/>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
@@ -3490,8 +3495,8 @@
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="12"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="31"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="14"/>
       <c r="E68" s="12"/>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
@@ -3510,8 +3515,8 @@
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="12"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="31"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="14"/>
       <c r="E69" s="12"/>
       <c r="F69" s="10"/>
       <c r="G69" s="10"/>
@@ -3530,8 +3535,8 @@
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="12"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="31"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="14"/>
       <c r="E70" s="12"/>
       <c r="F70" s="10"/>
       <c r="G70" s="10"/>
@@ -3550,8 +3555,8 @@
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="12"/>
-      <c r="C71" s="30"/>
-      <c r="D71" s="31"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="14"/>
       <c r="E71" s="12"/>
       <c r="F71" s="10"/>
       <c r="G71" s="10"/>
@@ -3570,8 +3575,8 @@
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="12"/>
-      <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="14"/>
       <c r="E72" s="12"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
@@ -3590,8 +3595,8 @@
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="12"/>
-      <c r="C73" s="30"/>
-      <c r="D73" s="31"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="14"/>
       <c r="E73" s="12"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
@@ -3610,8 +3615,8 @@
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="12"/>
-      <c r="C74" s="30"/>
-      <c r="D74" s="31"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="14"/>
       <c r="E74" s="12"/>
       <c r="F74" s="10"/>
       <c r="G74" s="10"/>
@@ -3630,8 +3635,8 @@
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="12"/>
-      <c r="C75" s="30"/>
-      <c r="D75" s="31"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="14"/>
       <c r="E75" s="12"/>
       <c r="F75" s="10"/>
       <c r="G75" s="10"/>
@@ -3650,8 +3655,8 @@
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="12"/>
-      <c r="C76" s="30"/>
-      <c r="D76" s="31"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="14"/>
       <c r="E76" s="12"/>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
@@ -3670,8 +3675,8 @@
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="12"/>
-      <c r="C77" s="30"/>
-      <c r="D77" s="31"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="14"/>
       <c r="E77" s="12"/>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
@@ -3690,8 +3695,8 @@
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="12"/>
-      <c r="C78" s="30"/>
-      <c r="D78" s="31"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="14"/>
       <c r="E78" s="12"/>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
@@ -3710,8 +3715,8 @@
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="12"/>
-      <c r="C79" s="30"/>
-      <c r="D79" s="31"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="14"/>
       <c r="E79" s="12"/>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
@@ -3730,8 +3735,8 @@
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="12"/>
-      <c r="C80" s="30"/>
-      <c r="D80" s="31"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="14"/>
       <c r="E80" s="12"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
@@ -3750,8 +3755,8 @@
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="12"/>
-      <c r="C81" s="30"/>
-      <c r="D81" s="31"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="14"/>
       <c r="E81" s="12"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
@@ -3770,8 +3775,8 @@
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="12"/>
-      <c r="C82" s="30"/>
-      <c r="D82" s="31"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="14"/>
       <c r="E82" s="12"/>
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
@@ -3790,8 +3795,8 @@
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="12"/>
-      <c r="C83" s="30"/>
-      <c r="D83" s="31"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="14"/>
       <c r="E83" s="12"/>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
@@ -3810,8 +3815,8 @@
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="12"/>
-      <c r="C84" s="30"/>
-      <c r="D84" s="31"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="14"/>
       <c r="E84" s="12"/>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
@@ -3830,8 +3835,8 @@
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="12"/>
-      <c r="C85" s="30"/>
-      <c r="D85" s="31"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="14"/>
       <c r="E85" s="12"/>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
@@ -3850,8 +3855,8 @@
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="12"/>
-      <c r="C86" s="30"/>
-      <c r="D86" s="31"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="14"/>
       <c r="E86" s="12"/>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
@@ -3870,8 +3875,8 @@
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="12"/>
-      <c r="C87" s="30"/>
-      <c r="D87" s="31"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="14"/>
       <c r="E87" s="12"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
@@ -3890,8 +3895,8 @@
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="12"/>
-      <c r="C88" s="30"/>
-      <c r="D88" s="31"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="14"/>
       <c r="E88" s="12"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
@@ -3910,8 +3915,8 @@
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="12"/>
-      <c r="C89" s="30"/>
-      <c r="D89" s="31"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="14"/>
       <c r="E89" s="12"/>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
@@ -3930,8 +3935,8 @@
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="12"/>
-      <c r="C90" s="30"/>
-      <c r="D90" s="31"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="14"/>
       <c r="E90" s="12"/>
       <c r="F90" s="10"/>
       <c r="G90" s="10"/>
@@ -3950,8 +3955,8 @@
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="12"/>
-      <c r="C91" s="30"/>
-      <c r="D91" s="31"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="14"/>
       <c r="E91" s="12"/>
       <c r="F91" s="10"/>
       <c r="G91" s="10"/>
@@ -3970,8 +3975,8 @@
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="12"/>
-      <c r="C92" s="30"/>
-      <c r="D92" s="31"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="14"/>
       <c r="E92" s="12"/>
       <c r="F92" s="10"/>
       <c r="G92" s="10"/>
@@ -3990,8 +3995,8 @@
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="12"/>
-      <c r="C93" s="30"/>
-      <c r="D93" s="31"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="14"/>
       <c r="E93" s="12"/>
       <c r="F93" s="10"/>
       <c r="G93" s="10"/>
@@ -4010,8 +4015,8 @@
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="12"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="31"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="14"/>
       <c r="E94" s="12"/>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
@@ -4030,8 +4035,8 @@
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="12"/>
-      <c r="C95" s="30"/>
-      <c r="D95" s="31"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="14"/>
       <c r="E95" s="12"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
@@ -6674,16 +6679,433 @@
     </row>
   </sheetData>
   <mergeCells count="475">
-    <mergeCell ref="I42:L42"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="P60:Q60"/>
+    <mergeCell ref="P61:Q61"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="P63:Q63"/>
+    <mergeCell ref="P64:Q64"/>
+    <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="P50:Q50"/>
+    <mergeCell ref="P51:Q51"/>
+    <mergeCell ref="P52:Q52"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="P54:Q54"/>
+    <mergeCell ref="P55:Q55"/>
+    <mergeCell ref="P56:Q56"/>
+    <mergeCell ref="P57:Q57"/>
+    <mergeCell ref="P42:Q42"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="P58:Q58"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="P84:Q84"/>
+    <mergeCell ref="P85:Q85"/>
+    <mergeCell ref="P93:Q93"/>
+    <mergeCell ref="P94:Q94"/>
+    <mergeCell ref="P95:Q95"/>
+    <mergeCell ref="P86:Q86"/>
+    <mergeCell ref="P87:Q87"/>
+    <mergeCell ref="P88:Q88"/>
+    <mergeCell ref="P89:Q89"/>
+    <mergeCell ref="P90:Q90"/>
+    <mergeCell ref="P91:Q91"/>
+    <mergeCell ref="P92:Q92"/>
+    <mergeCell ref="P75:Q75"/>
+    <mergeCell ref="P76:Q76"/>
+    <mergeCell ref="P77:Q77"/>
+    <mergeCell ref="P78:Q78"/>
+    <mergeCell ref="P79:Q79"/>
+    <mergeCell ref="P80:Q80"/>
+    <mergeCell ref="P81:Q81"/>
+    <mergeCell ref="P82:Q82"/>
+    <mergeCell ref="P83:Q83"/>
+    <mergeCell ref="P66:Q66"/>
+    <mergeCell ref="P67:Q67"/>
+    <mergeCell ref="P68:Q68"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="P70:Q70"/>
+    <mergeCell ref="P71:Q71"/>
+    <mergeCell ref="P72:Q72"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="P74:Q74"/>
+    <mergeCell ref="P65:Q65"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P22:Q22"/>
+    <mergeCell ref="P23:Q23"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="P30:Q30"/>
+    <mergeCell ref="P31:Q31"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="P35:Q35"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="P37:Q37"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="P40:Q40"/>
+    <mergeCell ref="P41:Q41"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="P15:Q15"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="I38:L38"/>
+    <mergeCell ref="I35:L35"/>
+    <mergeCell ref="I36:L36"/>
+    <mergeCell ref="I37:L37"/>
+    <mergeCell ref="I19:L19"/>
+    <mergeCell ref="I24:L24"/>
+    <mergeCell ref="I25:L25"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="I29:L29"/>
+    <mergeCell ref="I30:L30"/>
+    <mergeCell ref="I31:L31"/>
+    <mergeCell ref="I32:L32"/>
+    <mergeCell ref="I20:L20"/>
+    <mergeCell ref="I21:L21"/>
+    <mergeCell ref="I39:L39"/>
+    <mergeCell ref="I40:L40"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="I11:L11"/>
+    <mergeCell ref="I12:L12"/>
+    <mergeCell ref="I13:L13"/>
+    <mergeCell ref="I14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="I34:L34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="E18:H18"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="M52:O52"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="I43:L43"/>
+    <mergeCell ref="I44:L44"/>
+    <mergeCell ref="I45:L45"/>
+    <mergeCell ref="M53:O53"/>
+    <mergeCell ref="M54:O54"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E39:H39"/>
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="M64:O64"/>
+    <mergeCell ref="M65:O65"/>
+    <mergeCell ref="M66:O66"/>
+    <mergeCell ref="M67:O67"/>
+    <mergeCell ref="M68:O68"/>
+    <mergeCell ref="M69:O69"/>
+    <mergeCell ref="M90:O90"/>
+    <mergeCell ref="M91:O91"/>
+    <mergeCell ref="M92:O92"/>
+    <mergeCell ref="M70:O70"/>
+    <mergeCell ref="M71:O71"/>
+    <mergeCell ref="M72:O72"/>
+    <mergeCell ref="M82:O82"/>
+    <mergeCell ref="M73:O73"/>
+    <mergeCell ref="M74:O74"/>
+    <mergeCell ref="M75:O75"/>
+    <mergeCell ref="M76:O76"/>
+    <mergeCell ref="M77:O77"/>
+    <mergeCell ref="M78:O78"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="M80:O80"/>
+    <mergeCell ref="M81:O81"/>
+    <mergeCell ref="M93:O93"/>
+    <mergeCell ref="M94:O94"/>
+    <mergeCell ref="M95:O95"/>
+    <mergeCell ref="M83:O83"/>
+    <mergeCell ref="M84:O84"/>
+    <mergeCell ref="M85:O85"/>
+    <mergeCell ref="M86:O86"/>
+    <mergeCell ref="M87:O87"/>
+    <mergeCell ref="M88:O88"/>
+    <mergeCell ref="M89:O89"/>
+    <mergeCell ref="I60:L60"/>
+    <mergeCell ref="I61:L61"/>
+    <mergeCell ref="I62:L62"/>
+    <mergeCell ref="I63:L63"/>
+    <mergeCell ref="M55:O55"/>
+    <mergeCell ref="M56:O56"/>
+    <mergeCell ref="M57:O57"/>
+    <mergeCell ref="M58:O58"/>
+    <mergeCell ref="M59:O59"/>
+    <mergeCell ref="M60:O60"/>
+    <mergeCell ref="M61:O61"/>
+    <mergeCell ref="M62:O62"/>
+    <mergeCell ref="M63:O63"/>
+    <mergeCell ref="I51:L51"/>
+    <mergeCell ref="I52:L52"/>
+    <mergeCell ref="I53:L53"/>
+    <mergeCell ref="I54:L54"/>
+    <mergeCell ref="I55:L55"/>
+    <mergeCell ref="I56:L56"/>
+    <mergeCell ref="I57:L57"/>
+    <mergeCell ref="I58:L58"/>
+    <mergeCell ref="I59:L59"/>
+    <mergeCell ref="I22:L22"/>
+    <mergeCell ref="I23:L23"/>
+    <mergeCell ref="I82:L82"/>
+    <mergeCell ref="I83:L83"/>
+    <mergeCell ref="I84:L84"/>
+    <mergeCell ref="I92:L92"/>
+    <mergeCell ref="I93:L93"/>
+    <mergeCell ref="I73:L73"/>
+    <mergeCell ref="I74:L74"/>
+    <mergeCell ref="I75:L75"/>
+    <mergeCell ref="I76:L76"/>
+    <mergeCell ref="I77:L77"/>
+    <mergeCell ref="I78:L78"/>
+    <mergeCell ref="I79:L79"/>
+    <mergeCell ref="I80:L80"/>
+    <mergeCell ref="I81:L81"/>
+    <mergeCell ref="I46:L46"/>
+    <mergeCell ref="I47:L47"/>
+    <mergeCell ref="I48:L48"/>
+    <mergeCell ref="I49:L49"/>
+    <mergeCell ref="I50:L50"/>
+    <mergeCell ref="I33:L33"/>
+    <mergeCell ref="I72:L72"/>
+    <mergeCell ref="I41:L41"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="E45:H45"/>
+    <mergeCell ref="E46:H46"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E50:H50"/>
+    <mergeCell ref="I94:L94"/>
+    <mergeCell ref="I95:L95"/>
+    <mergeCell ref="I85:L85"/>
+    <mergeCell ref="I86:L86"/>
+    <mergeCell ref="I87:L87"/>
+    <mergeCell ref="I88:L88"/>
+    <mergeCell ref="I89:L89"/>
+    <mergeCell ref="I90:L90"/>
+    <mergeCell ref="I91:L91"/>
+    <mergeCell ref="I64:L64"/>
+    <mergeCell ref="I65:L65"/>
+    <mergeCell ref="I66:L66"/>
+    <mergeCell ref="I67:L67"/>
+    <mergeCell ref="I68:L68"/>
+    <mergeCell ref="I69:L69"/>
+    <mergeCell ref="I70:L70"/>
+    <mergeCell ref="I71:L71"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E53:H53"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="E43:H43"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="E33:H33"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E26:H26"/>
+    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E29:H29"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="E37:H37"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E94:H94"/>
+    <mergeCell ref="E95:H95"/>
+    <mergeCell ref="E89:H89"/>
+    <mergeCell ref="E90:H90"/>
+    <mergeCell ref="E91:H91"/>
+    <mergeCell ref="E92:H92"/>
+    <mergeCell ref="E93:H93"/>
+    <mergeCell ref="E84:H84"/>
+    <mergeCell ref="E85:H85"/>
+    <mergeCell ref="E86:H86"/>
+    <mergeCell ref="E87:H87"/>
+    <mergeCell ref="E88:H88"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="E77:H77"/>
+    <mergeCell ref="E78:H78"/>
+    <mergeCell ref="E79:H79"/>
+    <mergeCell ref="E80:H80"/>
+    <mergeCell ref="E81:H81"/>
+    <mergeCell ref="E73:H73"/>
+    <mergeCell ref="E74:H74"/>
+    <mergeCell ref="E66:H66"/>
+    <mergeCell ref="E67:H67"/>
+    <mergeCell ref="E68:H68"/>
+    <mergeCell ref="E69:H69"/>
+    <mergeCell ref="E70:H70"/>
+    <mergeCell ref="E71:H71"/>
+    <mergeCell ref="E72:H72"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E55:H55"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="E22:H22"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="E25:H25"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E44:H44"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B2:D2"/>
@@ -6708,30 +7130,16 @@
     <mergeCell ref="B69:D69"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E55:H55"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E24:H24"/>
-    <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E44:H44"/>
+    <mergeCell ref="I42:L42"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B90:D90"/>
     <mergeCell ref="E56:H56"/>
     <mergeCell ref="E64:H64"/>
     <mergeCell ref="E65:H65"/>
@@ -6746,409 +7154,6 @@
     <mergeCell ref="E83:H83"/>
     <mergeCell ref="E75:H75"/>
     <mergeCell ref="E76:H76"/>
-    <mergeCell ref="E77:H77"/>
-    <mergeCell ref="E78:H78"/>
-    <mergeCell ref="E79:H79"/>
-    <mergeCell ref="E80:H80"/>
-    <mergeCell ref="E81:H81"/>
-    <mergeCell ref="E73:H73"/>
-    <mergeCell ref="E74:H74"/>
-    <mergeCell ref="E66:H66"/>
-    <mergeCell ref="E67:H67"/>
-    <mergeCell ref="E68:H68"/>
-    <mergeCell ref="E69:H69"/>
-    <mergeCell ref="E70:H70"/>
-    <mergeCell ref="E71:H71"/>
-    <mergeCell ref="E72:H72"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="E94:H94"/>
-    <mergeCell ref="E95:H95"/>
-    <mergeCell ref="E89:H89"/>
-    <mergeCell ref="E90:H90"/>
-    <mergeCell ref="E91:H91"/>
-    <mergeCell ref="E92:H92"/>
-    <mergeCell ref="E93:H93"/>
-    <mergeCell ref="E84:H84"/>
-    <mergeCell ref="E85:H85"/>
-    <mergeCell ref="E86:H86"/>
-    <mergeCell ref="E87:H87"/>
-    <mergeCell ref="E88:H88"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E3:H3"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="E5:H5"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="E53:H53"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="E43:H43"/>
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E33:H33"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E26:H26"/>
-    <mergeCell ref="E27:H27"/>
-    <mergeCell ref="E28:H28"/>
-    <mergeCell ref="E29:H29"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="E36:H36"/>
-    <mergeCell ref="E37:H37"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="E45:H45"/>
-    <mergeCell ref="E46:H46"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E50:H50"/>
-    <mergeCell ref="I94:L94"/>
-    <mergeCell ref="I95:L95"/>
-    <mergeCell ref="I85:L85"/>
-    <mergeCell ref="I86:L86"/>
-    <mergeCell ref="I87:L87"/>
-    <mergeCell ref="I88:L88"/>
-    <mergeCell ref="I89:L89"/>
-    <mergeCell ref="I90:L90"/>
-    <mergeCell ref="I91:L91"/>
-    <mergeCell ref="I22:L22"/>
-    <mergeCell ref="I23:L23"/>
-    <mergeCell ref="I82:L82"/>
-    <mergeCell ref="I83:L83"/>
-    <mergeCell ref="I84:L84"/>
-    <mergeCell ref="I92:L92"/>
-    <mergeCell ref="I93:L93"/>
-    <mergeCell ref="I73:L73"/>
-    <mergeCell ref="I74:L74"/>
-    <mergeCell ref="I75:L75"/>
-    <mergeCell ref="I76:L76"/>
-    <mergeCell ref="I77:L77"/>
-    <mergeCell ref="I78:L78"/>
-    <mergeCell ref="I79:L79"/>
-    <mergeCell ref="I80:L80"/>
-    <mergeCell ref="I81:L81"/>
-    <mergeCell ref="I46:L46"/>
-    <mergeCell ref="I47:L47"/>
-    <mergeCell ref="I48:L48"/>
-    <mergeCell ref="I49:L49"/>
-    <mergeCell ref="I50:L50"/>
-    <mergeCell ref="I33:L33"/>
-    <mergeCell ref="I72:L72"/>
-    <mergeCell ref="I41:L41"/>
-    <mergeCell ref="I64:L64"/>
-    <mergeCell ref="I65:L65"/>
-    <mergeCell ref="I66:L66"/>
-    <mergeCell ref="I67:L67"/>
-    <mergeCell ref="I68:L68"/>
-    <mergeCell ref="I69:L69"/>
-    <mergeCell ref="I70:L70"/>
-    <mergeCell ref="I71:L71"/>
-    <mergeCell ref="I51:L51"/>
-    <mergeCell ref="I52:L52"/>
-    <mergeCell ref="I53:L53"/>
-    <mergeCell ref="I54:L54"/>
-    <mergeCell ref="I55:L55"/>
-    <mergeCell ref="I56:L56"/>
-    <mergeCell ref="I57:L57"/>
-    <mergeCell ref="I58:L58"/>
-    <mergeCell ref="I59:L59"/>
-    <mergeCell ref="I60:L60"/>
-    <mergeCell ref="I61:L61"/>
-    <mergeCell ref="I62:L62"/>
-    <mergeCell ref="I63:L63"/>
-    <mergeCell ref="M55:O55"/>
-    <mergeCell ref="M56:O56"/>
-    <mergeCell ref="M57:O57"/>
-    <mergeCell ref="M58:O58"/>
-    <mergeCell ref="M59:O59"/>
-    <mergeCell ref="M60:O60"/>
-    <mergeCell ref="M61:O61"/>
-    <mergeCell ref="M62:O62"/>
-    <mergeCell ref="M63:O63"/>
-    <mergeCell ref="M93:O93"/>
-    <mergeCell ref="M94:O94"/>
-    <mergeCell ref="M95:O95"/>
-    <mergeCell ref="M83:O83"/>
-    <mergeCell ref="M84:O84"/>
-    <mergeCell ref="M85:O85"/>
-    <mergeCell ref="M86:O86"/>
-    <mergeCell ref="M87:O87"/>
-    <mergeCell ref="M88:O88"/>
-    <mergeCell ref="M89:O89"/>
-    <mergeCell ref="M64:O64"/>
-    <mergeCell ref="M65:O65"/>
-    <mergeCell ref="M66:O66"/>
-    <mergeCell ref="M67:O67"/>
-    <mergeCell ref="M68:O68"/>
-    <mergeCell ref="M69:O69"/>
-    <mergeCell ref="M90:O90"/>
-    <mergeCell ref="M91:O91"/>
-    <mergeCell ref="M92:O92"/>
-    <mergeCell ref="M70:O70"/>
-    <mergeCell ref="M71:O71"/>
-    <mergeCell ref="M72:O72"/>
-    <mergeCell ref="M82:O82"/>
-    <mergeCell ref="M73:O73"/>
-    <mergeCell ref="M74:O74"/>
-    <mergeCell ref="M75:O75"/>
-    <mergeCell ref="M76:O76"/>
-    <mergeCell ref="M77:O77"/>
-    <mergeCell ref="M78:O78"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="M80:O80"/>
-    <mergeCell ref="M81:O81"/>
-    <mergeCell ref="I43:L43"/>
-    <mergeCell ref="I44:L44"/>
-    <mergeCell ref="I45:L45"/>
-    <mergeCell ref="M53:O53"/>
-    <mergeCell ref="M54:O54"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E39:H39"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="E41:H41"/>
-    <mergeCell ref="E42:H42"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="M52:O52"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="E18:H18"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I39:L39"/>
-    <mergeCell ref="I40:L40"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="I11:L11"/>
-    <mergeCell ref="I12:L12"/>
-    <mergeCell ref="I13:L13"/>
-    <mergeCell ref="I14:L14"/>
-    <mergeCell ref="I15:L15"/>
-    <mergeCell ref="I16:L16"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="I18:L18"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="I34:L34"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="P12:Q12"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="P15:Q15"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="P18:Q18"/>
-    <mergeCell ref="I38:L38"/>
-    <mergeCell ref="I35:L35"/>
-    <mergeCell ref="I36:L36"/>
-    <mergeCell ref="I37:L37"/>
-    <mergeCell ref="I19:L19"/>
-    <mergeCell ref="I24:L24"/>
-    <mergeCell ref="I25:L25"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="I29:L29"/>
-    <mergeCell ref="I30:L30"/>
-    <mergeCell ref="I31:L31"/>
-    <mergeCell ref="I32:L32"/>
-    <mergeCell ref="I20:L20"/>
-    <mergeCell ref="I21:L21"/>
-    <mergeCell ref="P65:Q65"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P22:Q22"/>
-    <mergeCell ref="P23:Q23"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="P30:Q30"/>
-    <mergeCell ref="P31:Q31"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="P35:Q35"/>
-    <mergeCell ref="P36:Q36"/>
-    <mergeCell ref="P37:Q37"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="P40:Q40"/>
-    <mergeCell ref="P41:Q41"/>
-    <mergeCell ref="P66:Q66"/>
-    <mergeCell ref="P67:Q67"/>
-    <mergeCell ref="P68:Q68"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="P70:Q70"/>
-    <mergeCell ref="P71:Q71"/>
-    <mergeCell ref="P72:Q72"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="P74:Q74"/>
-    <mergeCell ref="P75:Q75"/>
-    <mergeCell ref="P76:Q76"/>
-    <mergeCell ref="P77:Q77"/>
-    <mergeCell ref="P78:Q78"/>
-    <mergeCell ref="P79:Q79"/>
-    <mergeCell ref="P80:Q80"/>
-    <mergeCell ref="P81:Q81"/>
-    <mergeCell ref="P82:Q82"/>
-    <mergeCell ref="P83:Q83"/>
-    <mergeCell ref="P84:Q84"/>
-    <mergeCell ref="P85:Q85"/>
-    <mergeCell ref="P93:Q93"/>
-    <mergeCell ref="P94:Q94"/>
-    <mergeCell ref="P95:Q95"/>
-    <mergeCell ref="P86:Q86"/>
-    <mergeCell ref="P87:Q87"/>
-    <mergeCell ref="P88:Q88"/>
-    <mergeCell ref="P89:Q89"/>
-    <mergeCell ref="P90:Q90"/>
-    <mergeCell ref="P91:Q91"/>
-    <mergeCell ref="P92:Q92"/>
-    <mergeCell ref="P42:Q42"/>
-    <mergeCell ref="P43:Q43"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="P58:Q58"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="P60:Q60"/>
-    <mergeCell ref="P61:Q61"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="P63:Q63"/>
-    <mergeCell ref="P64:Q64"/>
-    <mergeCell ref="P49:Q49"/>
-    <mergeCell ref="P50:Q50"/>
-    <mergeCell ref="P51:Q51"/>
-    <mergeCell ref="P52:Q52"/>
-    <mergeCell ref="P53:Q53"/>
-    <mergeCell ref="P54:Q54"/>
-    <mergeCell ref="P55:Q55"/>
-    <mergeCell ref="P56:Q56"/>
-    <mergeCell ref="P57:Q57"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="M17:O17"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Doc: Updated Regiteration and supplier feature in CRS,SRS and RTM according to assessment comments
</commit_message>
<xml_diff>
--- a/Test/Test-cases.xlsx
+++ b/Test/Test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F834F67-1E54-494C-909A-5ACDDFE7F581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A8B25-1F6D-45CE-8D06-84A8560A80F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="385">
   <si>
     <t>Test case ID</t>
   </si>
@@ -1261,6 +1261,414 @@
   </si>
   <si>
     <t>Platform:""</t>
+  </si>
+  <si>
+    <t>TC_Register_018</t>
+  </si>
+  <si>
+    <t>Verify username field is mandatory</t>
+  </si>
+  <si>
+    <t>Registration page is open</t>
+  </si>
+  <si>
+    <t>1. Open registration page
+2. Leave all fields empty
+3. Click "Register" button</t>
+  </si>
+  <si>
+    <t>All fields empty</t>
+  </si>
+  <si>
+    <t>TC_Register_019</t>
+  </si>
+  <si>
+    <t>Validate username with special characters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields with valid data
+2. Use Test@User! as username
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Username = Test@User!
+Email = test@example.com
+Password = Pass1234
+Confirm = Pass1234
+Address = Cairo
+Phone = +201234567890
+National ID = 12345678901234</t>
+  </si>
+  <si>
+    <t>TC_Register_020</t>
+  </si>
+  <si>
+    <t>Validate username with mixed-case letters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use TestUser as username
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Username = TestUser
+Email = testuser@example.com
+Password = Pass1234
+Confirm = Pass1234
+Address = Alex
+Phone = +201234567890
+National ID = 12345678901234</t>
+  </si>
+  <si>
+    <t>Registration successful</t>
+  </si>
+  <si>
+    <t>TC_Register_021</t>
+  </si>
+  <si>
+    <t>Validate email with uppercase letters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use TEST@EMAIL.COM
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Username = mariam123
+Email = TEST@EMAIL.COM
+Password = Test1234
+Confirm = Test1234
+Address = Nasr City
+Phone = +201111223344
+National ID = 12345678901234</t>
+  </si>
+  <si>
+    <t>TC_Register_022</t>
+  </si>
+  <si>
+    <t>Validate password with exactly 8 characters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use Abcd1234 as password
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Password = Abcd1234
+Confirm = Abcd1234
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_023</t>
+  </si>
+  <si>
+    <t>Validate password with special characters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use Pa$$word!
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Password = Pa$$word!
+Confirm = Pa$$word!
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_024</t>
+  </si>
+  <si>
+    <t>Validate address with only numbers</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use 123456 as address
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Address = 123456
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_025</t>
+  </si>
+  <si>
+    <t>Validate address with only letters</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use MainStreet as address
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Address = MainStreet
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_026</t>
+  </si>
+  <si>
+    <t>Validate phone with 10 digits after +20</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use +201234567893 as phone
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Phone = +2012345678901
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_027</t>
+  </si>
+  <si>
+    <t>Validate phone with more than 10 digits</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use +201234567890123
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Phone = +201234567890123
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_028</t>
+  </si>
+  <si>
+    <t>Validate National ID with 13 digits</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use 1234567890123
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>National ID = 1234567890123
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_029</t>
+  </si>
+  <si>
+    <t>Validate National ID with 15 digits</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use 123456789012345
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>National ID = 123456789012345
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Register_030</t>
+  </si>
+  <si>
+    <t>Validate inputs with leading/trailing spaces</t>
+  </si>
+  <si>
+    <t>1. Fill all fields
+2. Use " Mariam " as username
+3. Click "Register"</t>
+  </si>
+  <si>
+    <t>Username = Mariam
+All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Supplier_009</t>
+  </si>
+  <si>
+    <t>Validate adding product with empty Product ID</t>
+  </si>
+  <si>
+    <t>Add Product page open</t>
+  </si>
+  <si>
+    <t>1. Leave Product ID empty
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: (empty)
+Price: 500
+Version: 1.0.0
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>Error message: "Invalid Data"</t>
+  </si>
+  <si>
+    <t>https://share.balsamiq.com/c/gSAJhmDq1Ff3FhHi1LzTBS.jpg</t>
+  </si>
+  <si>
+    <t>TC_Supplier_010</t>
+  </si>
+  <si>
+    <t>Validate Product ID with wrong format</t>
+  </si>
+  <si>
+    <t>1. Enter Shoes42 in Product ID
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Shoes42
+Price: 500
+Version: 1.0.0
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>Error message: "Invalid Product ID"</t>
+  </si>
+  <si>
+    <t>TC_Supplier_011</t>
+  </si>
+  <si>
+    <t>Validate empty Product Photo</t>
+  </si>
+  <si>
+    <t>1. Leave product photo empty
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>TC_Supplier_012</t>
+  </si>
+  <si>
+    <t>Validate empty Product Price</t>
+  </si>
+  <si>
+    <t>1. Leave Price field empty
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Nike_Shoes_42
+Price: (empty)
+Version: 1.0.0
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>TC_Supplier_013</t>
+  </si>
+  <si>
+    <t>Validate Product Price with special characters</t>
+  </si>
+  <si>
+    <t>1. Enter $500 in Price
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Nike_Shoes_42
+Price: $500
+Version: 1.0.0
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>TC_Supplier_014</t>
+  </si>
+  <si>
+    <t>Validate empty Version field</t>
+  </si>
+  <si>
+    <t>1. Leave Version empty
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Nike_Shoes_42
+Price: 500
+Version: (empty)
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>TC_Supplier_015</t>
+  </si>
+  <si>
+    <t>Validate malformed Version (e.g. 1..0)</t>
+  </si>
+  <si>
+    <t>1. Enter 1..0 as Version
+2. Fill other fields
+3. Click "Add product"</t>
+  </si>
+  <si>
+    <t>Product ID: Nike_Shoes_42
+Price: 500
+Version: 1..0
+Platform: Android
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>TC_Supplier_016</t>
+  </si>
+  <si>
+    <t>Validate invalid Platform option</t>
+  </si>
+  <si>
+    <t>1. Try to type "Windows" in platform field
+2. Fill other fields
+3. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Nike_Shoes_42
+Price: 500
+Version: 1.0.0
+Platform: Windows
+Image: 250KB</t>
+  </si>
+  <si>
+    <t>TC_Supplier_017</t>
+  </si>
+  <si>
+    <t>Submit empty form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Add Product page open</t>
+  </si>
+  <si>
+    <t>1. Leave all fields empty
+2. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: (empty)
+Price: (empty)
+Version: (empty)
+Platform: (empty)
+Image: (empty)</t>
+  </si>
+  <si>
+    <t>TC_Supplier_018</t>
+  </si>
+  <si>
+    <t>Submit with multiple invalid fields</t>
+  </si>
+  <si>
+    <t>1. Enter invalid ID Shoes42
+2. Upload 400KB image
+3. Enter $700 as price
+4. Click "Add Product"</t>
+  </si>
+  <si>
+    <t>Product ID: Shoes42
+Price: $700
+Version: 1.0.0
+Platform: Android
+Image: 400KB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message: "Invalid Data"	</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1544,13 +1952,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1636,7 +2055,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1654,6 +2072,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1874,10 +2313,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J967"/>
+  <dimension ref="A1:J990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="62" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="62" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1910,10 +2349,10 @@
       <c r="E1" s="33" t="s">
         <v>196</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -1940,7 +2379,7 @@
       <c r="F2" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="47"/>
+      <c r="G2" s="46"/>
       <c r="H2" s="42"/>
       <c r="I2" s="10" t="s">
         <v>180</v>
@@ -1963,7 +2402,7 @@
       <c r="F3" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="46"/>
       <c r="H3" s="42"/>
       <c r="I3" s="10" t="s">
         <v>162</v>
@@ -1986,7 +2425,7 @@
       <c r="F4" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="42"/>
       <c r="I4" s="11" t="s">
         <v>174</v>
@@ -2009,7 +2448,7 @@
       <c r="F5" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="42"/>
       <c r="I5" s="11" t="s">
         <v>173</v>
@@ -2029,10 +2468,10 @@
         <v>73</v>
       </c>
       <c r="E6" s="39"/>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="46"/>
       <c r="H6" s="42"/>
       <c r="I6" s="11" t="s">
         <v>172</v>
@@ -2052,10 +2491,10 @@
         <v>161</v>
       </c>
       <c r="E7" s="39"/>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="47"/>
+      <c r="G7" s="46"/>
       <c r="H7" s="42"/>
       <c r="I7" s="11" t="s">
         <v>163</v>
@@ -2078,7 +2517,7 @@
       <c r="F8" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G8" s="47"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="42"/>
       <c r="I8" s="11" t="s">
         <v>171</v>
@@ -2098,10 +2537,10 @@
         <v>83</v>
       </c>
       <c r="E9" s="39"/>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="47"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="42"/>
       <c r="I9" s="11" t="s">
         <v>163</v>
@@ -2124,7 +2563,7 @@
       <c r="F10" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="G10" s="47"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="42"/>
       <c r="I10" s="11" t="s">
         <v>170</v>
@@ -2147,7 +2586,7 @@
       <c r="F11" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="G11" s="47"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="42"/>
       <c r="I11" s="11" t="s">
         <v>169</v>
@@ -2170,7 +2609,7 @@
       <c r="F12" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="G12" s="47"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="42"/>
       <c r="I12" s="11" t="s">
         <v>168</v>
@@ -2190,10 +2629,10 @@
         <v>96</v>
       </c>
       <c r="E13" s="39"/>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G13" s="47"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="42"/>
       <c r="I13" s="11" t="s">
         <v>167</v>
@@ -2213,10 +2652,10 @@
         <v>99</v>
       </c>
       <c r="E14" s="39"/>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G14" s="47"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="42"/>
       <c r="I14" s="11" t="s">
         <v>166</v>
@@ -2236,10 +2675,10 @@
         <v>99</v>
       </c>
       <c r="E15" s="39"/>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="47"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="42"/>
       <c r="I15" s="11" t="s">
         <v>163</v>
@@ -2259,10 +2698,10 @@
         <v>105</v>
       </c>
       <c r="E16" s="39"/>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="47"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="42"/>
       <c r="I16" s="11" t="s">
         <v>165</v>
@@ -2282,10 +2721,10 @@
         <v>108</v>
       </c>
       <c r="E17" s="39"/>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="47"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="42"/>
       <c r="I17" s="11" t="s">
         <v>164</v>
@@ -2305,1384 +2744,1855 @@
         <v>111</v>
       </c>
       <c r="E18" s="39"/>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="47"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="11" t="s">
+      <c r="G18" s="53"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="55" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="49"/>
-      <c r="H19" s="43"/>
-    </row>
-    <row r="20" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="47"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="12" t="s">
-        <v>191</v>
-      </c>
+    <row r="19" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>289</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>290</v>
+      </c>
+      <c r="F19" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="46"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="1:9" s="60" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="B20" s="56" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>293</v>
+      </c>
+      <c r="E20" s="58" t="s">
+        <v>294</v>
+      </c>
+      <c r="F20" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" s="31"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>295</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>44</v>
+        <v>296</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="47"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G21" s="46"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="11"/>
     </row>
     <row r="22" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>300</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>304</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>46</v>
+        <v>305</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="47"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="F23" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G23" s="46"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="11"/>
     </row>
     <row r="24" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>308</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>47</v>
+        <v>309</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="47"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="11" t="s">
-        <v>193</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G24" s="46"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="11"/>
     </row>
     <row r="25" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>312</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>48</v>
+        <v>313</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="G25" s="47"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="11" t="s">
-        <v>194</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="11"/>
     </row>
     <row r="26" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>316</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>49</v>
+        <v>317</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="47"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="11" t="s">
-        <v>195</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="F26" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G26" s="46"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>320</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>54</v>
+        <v>321</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="47"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="11" t="s">
-        <v>181</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="F27" s="47" t="s">
+        <v>299</v>
+      </c>
+      <c r="G27" s="46"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>324</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>50</v>
+        <v>325</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G28" s="47"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>326</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="11"/>
     </row>
     <row r="29" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>328</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>51</v>
+        <v>329</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="46"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="11"/>
     </row>
     <row r="30" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>332</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>52</v>
+        <v>333</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="47"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="11" t="s">
-        <v>192</v>
-      </c>
+        <v>288</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G30" s="46"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="11"/>
     </row>
     <row r="31" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>336</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>53</v>
+        <v>337</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="47"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="11" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="46"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="11"/>
+    </row>
+    <row r="32" spans="1:9" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33" s="46"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G33" s="47"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="11" t="s">
+      <c r="G34" s="46"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="11" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>280</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>281</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E35" s="39"/>
       <c r="F35" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="G35" s="47"/>
+        <v>21</v>
+      </c>
+      <c r="G35" s="46"/>
       <c r="H35" s="36"/>
       <c r="I35" s="11" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>276</v>
-      </c>
-      <c r="E36" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="F36" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="G36" s="47"/>
+        <v>12</v>
+      </c>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="46"/>
       <c r="H36" s="36"/>
       <c r="I36" s="11" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>123</v>
+        <v>47</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>124</v>
+        <v>13</v>
       </c>
       <c r="E37" s="39"/>
       <c r="F37" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="G37" s="47"/>
+        <v>22</v>
+      </c>
+      <c r="G37" s="46"/>
       <c r="H37" s="36"/>
       <c r="I37" s="11" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>125</v>
+        <v>32</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>126</v>
+        <v>48</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>277</v>
-      </c>
-      <c r="E38" s="39" t="s">
-        <v>283</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E38" s="39"/>
       <c r="F38" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="47"/>
+        <v>23</v>
+      </c>
+      <c r="G38" s="46"/>
       <c r="H38" s="36"/>
       <c r="I38" s="11" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>127</v>
+        <v>33</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>128</v>
+        <v>49</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D39" s="39" t="s">
-        <v>278</v>
-      </c>
-      <c r="E39" s="39" t="s">
-        <v>284</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E39" s="39"/>
       <c r="F39" s="39" t="s">
-        <v>158</v>
-      </c>
-      <c r="G39" s="47"/>
+        <v>24</v>
+      </c>
+      <c r="G39" s="46"/>
       <c r="H39" s="36"/>
       <c r="I39" s="11" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="6" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>129</v>
+        <v>34</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>120</v>
+        <v>8</v>
       </c>
       <c r="D40" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>285</v>
-      </c>
-      <c r="F40" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="G40" s="47"/>
+        <v>16</v>
+      </c>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="46"/>
       <c r="H40" s="36"/>
       <c r="I40" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="32" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>132</v>
+        <v>35</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>133</v>
+        <v>50</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="D41" s="39" t="s">
-        <v>279</v>
-      </c>
-      <c r="E41" s="39" t="s">
-        <v>281</v>
-      </c>
-      <c r="F41" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="G41" s="47"/>
+        <v>17</v>
+      </c>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G41" s="46"/>
       <c r="H41" s="36"/>
       <c r="I41" s="11" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="32" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>136</v>
+        <v>36</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>134</v>
+        <v>8</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="E42" s="39" t="s">
-        <v>282</v>
-      </c>
-      <c r="F42" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="46"/>
       <c r="H42" s="36"/>
       <c r="I42" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="32" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="46"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="32" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" s="46"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="J44" s="19"/>
+    </row>
+    <row r="45" spans="1:10" s="32" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="G45" s="46"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="J45" s="19"/>
+    </row>
+    <row r="46" spans="1:10" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="46"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="J46" s="19"/>
+    </row>
+    <row r="47" spans="1:10" s="32" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" s="32" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="E48" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="F48" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="G48" s="46"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="32" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49" s="39" t="s">
+        <v>276</v>
+      </c>
+      <c r="E49" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="F49" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="46"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="J49" s="19"/>
+    </row>
+    <row r="50" spans="1:10" s="32" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G50" s="46"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="32" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="E51" s="39" t="s">
+        <v>283</v>
+      </c>
+      <c r="F51" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" s="46"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="32" customFormat="1" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="E52" s="39" t="s">
+        <v>284</v>
+      </c>
+      <c r="F52" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="G52" s="46"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="32" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D53" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="39" t="s">
+        <v>285</v>
+      </c>
+      <c r="F53" s="49" t="s">
+        <v>158</v>
+      </c>
+      <c r="G53" s="46"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="32" customFormat="1" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="39" t="s">
+        <v>279</v>
+      </c>
+      <c r="E54" s="39" t="s">
+        <v>281</v>
+      </c>
+      <c r="F54" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G54" s="46"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" s="32" customFormat="1" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" s="39" t="s">
+        <v>282</v>
+      </c>
+      <c r="F55" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G55" s="46"/>
+      <c r="H55" s="36"/>
+      <c r="I55" s="11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="22"/>
-    </row>
-    <row r="44" spans="1:10" s="32" customFormat="1" ht="84.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="s">
+    <row r="56" spans="1:10" s="32" customFormat="1" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D56" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="F56" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G56" s="46"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D57" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="F57" s="47" t="s">
+        <v>351</v>
+      </c>
+      <c r="G57" s="46"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" s="32" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D58" s="39" t="s">
+        <v>354</v>
+      </c>
+      <c r="E58" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="F58" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G58" s="46"/>
+      <c r="H58" s="36"/>
+      <c r="I58" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="32" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D59" s="39" t="s">
+        <v>357</v>
+      </c>
+      <c r="E59" s="39" t="s">
+        <v>358</v>
+      </c>
+      <c r="F59" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G59" s="46"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="32" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B60" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D60" s="39" t="s">
+        <v>361</v>
+      </c>
+      <c r="E60" s="39" t="s">
+        <v>362</v>
+      </c>
+      <c r="F60" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G60" s="46"/>
+      <c r="H60" s="36"/>
+      <c r="I60" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" s="32" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B61" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>365</v>
+      </c>
+      <c r="E61" s="39" t="s">
+        <v>366</v>
+      </c>
+      <c r="F61" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G61" s="46"/>
+      <c r="H61" s="36"/>
+      <c r="I61" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B62" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D62" s="39" t="s">
+        <v>369</v>
+      </c>
+      <c r="E62" s="39" t="s">
+        <v>370</v>
+      </c>
+      <c r="F62" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G62" s="46"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B63" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D63" s="39" t="s">
+        <v>373</v>
+      </c>
+      <c r="E63" s="39" t="s">
+        <v>374</v>
+      </c>
+      <c r="F63" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G63" s="46"/>
+      <c r="H63" s="36"/>
+      <c r="I63" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="C64" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="D64" s="39" t="s">
+        <v>378</v>
+      </c>
+      <c r="E64" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="F64" s="47" t="s">
+        <v>345</v>
+      </c>
+      <c r="G64" s="46"/>
+      <c r="H64" s="36"/>
+      <c r="I64" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B65" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="D65" s="39" t="s">
+        <v>382</v>
+      </c>
+      <c r="E65" s="39" t="s">
+        <v>383</v>
+      </c>
+      <c r="F65" s="47" t="s">
+        <v>384</v>
+      </c>
+      <c r="G65" s="46"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="11" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="40"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="40"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="22"/>
+    </row>
+    <row r="67" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B67" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C67" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D67" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E67" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F67" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="G44" s="31"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="18" t="s">
+      <c r="G67" s="31"/>
+      <c r="H67" s="43"/>
+      <c r="I67" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="32" customFormat="1" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+    <row r="68" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B68" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C68" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D45" s="29" t="s">
+      <c r="D68" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E45" s="30" t="s">
+      <c r="E68" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="F45" s="29" t="s">
+      <c r="F68" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="G45" s="31"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="18" t="s">
+      <c r="G68" s="31"/>
+      <c r="H68" s="43"/>
+      <c r="I68" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="32" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+    <row r="69" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B69" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C69" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D69" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="E69" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="F46" s="29" t="s">
+      <c r="F69" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="G46" s="31"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="18" t="s">
+      <c r="G69" s="31"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="32" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+    <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B70" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C70" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D47" s="29" t="s">
+      <c r="D70" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="30" t="s">
+      <c r="E70" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="F47" s="29" t="s">
+      <c r="F70" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="G47" s="31"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="18" t="s">
+      <c r="G70" s="31"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="J47" s="19"/>
-    </row>
-    <row r="48" spans="1:10" s="32" customFormat="1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+    </row>
+    <row r="71" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B71" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C71" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D48" s="29" t="s">
+      <c r="D71" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="E71" s="30" t="s">
         <v>230</v>
       </c>
-      <c r="F48" s="29" t="s">
+      <c r="F71" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="G48" s="31"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="18" t="s">
+      <c r="G71" s="31"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="J48" s="19"/>
-    </row>
-    <row r="49" spans="1:10" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+    </row>
+    <row r="72" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B72" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C72" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D49" s="29" t="s">
+      <c r="D72" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="E72" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="F72" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="G49" s="31"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="18" t="s">
+      <c r="G72" s="31"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="J49" s="19"/>
-    </row>
-    <row r="50" spans="1:10" s="32" customFormat="1" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+    </row>
+    <row r="73" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B73" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C73" s="35" t="s">
         <v>222</v>
       </c>
-      <c r="D50" s="29" t="s">
+      <c r="D73" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="E73" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F73" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="G50" s="31"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="18" t="s">
+      <c r="G73" s="31"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="32" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+    <row r="74" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B74" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C74" s="35" t="s">
         <v>236</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="D74" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="E74" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="F51" s="29" t="s">
+      <c r="F74" s="29" t="s">
         <v>274</v>
       </c>
-      <c r="G51" s="31"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="18" t="s">
+      <c r="G74" s="31"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="18" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="32" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="s">
+    <row r="75" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B75" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C75" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="D75" s="29" t="s">
         <v>239</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="E75" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F75" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="G52" s="31"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="19" t="s">
+      <c r="G75" s="31"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="J52" s="19"/>
-    </row>
-    <row r="53" spans="1:10" s="32" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+    </row>
+    <row r="76" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B76" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C76" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="D76" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="E76" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F76" s="29" t="s">
         <v>245</v>
       </c>
-      <c r="G53" s="31"/>
-      <c r="H53" s="44"/>
-      <c r="I53" s="19" t="s">
+      <c r="G76" s="31"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="32" customFormat="1" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+    <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B77" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C77" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="D77" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E77" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F77" s="29" t="s">
         <v>247</v>
       </c>
-      <c r="G54" s="31"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="19" t="s">
+      <c r="G77" s="31"/>
+      <c r="H77" s="43"/>
+      <c r="I77" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="32" customFormat="1" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
+    <row r="78" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B78" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C78" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="D78" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E78" s="30" t="s">
         <v>248</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F78" s="29" t="s">
         <v>249</v>
       </c>
-      <c r="G55" s="31"/>
-      <c r="H55" s="44"/>
-      <c r="I55" s="19" t="s">
+      <c r="G78" s="31"/>
+      <c r="H78" s="43"/>
+      <c r="I78" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="32" customFormat="1" ht="75.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="s">
+    <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B79" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C79" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D56" s="29" t="s">
+      <c r="D79" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="E79" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F79" s="29" t="s">
         <v>250</v>
       </c>
-      <c r="G56" s="31"/>
-      <c r="H56" s="44"/>
-      <c r="I56" s="19" t="s">
+      <c r="G79" s="31"/>
+      <c r="H79" s="43"/>
+      <c r="I79" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="32" customFormat="1" ht="107.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+    <row r="80" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B80" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C80" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D57" s="29" t="s">
+      <c r="D80" s="29" t="s">
         <v>251</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="E80" s="30" t="s">
         <v>252</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F80" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="G57" s="31"/>
-      <c r="H57" s="44"/>
-      <c r="I57" s="19" t="s">
+      <c r="G80" s="31"/>
+      <c r="H80" s="43"/>
+      <c r="I80" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="32" customFormat="1" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+    <row r="81" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B81" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C81" s="35" t="s">
         <v>254</v>
       </c>
-      <c r="D58" s="29" t="s">
+      <c r="D81" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="E81" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F81" s="29" t="s">
         <v>257</v>
       </c>
-      <c r="G58" s="31"/>
-      <c r="H58" s="44"/>
-      <c r="I58" s="19" t="s">
+      <c r="G81" s="31"/>
+      <c r="H81" s="43"/>
+      <c r="I81" s="19" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="32" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+    <row r="82" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B82" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="C59" s="35" t="s">
+      <c r="C82" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D59" s="29" t="s">
+      <c r="D82" s="29" t="s">
         <v>258</v>
       </c>
-      <c r="E59" s="30" t="s">
+      <c r="E82" s="30" t="s">
         <v>259</v>
       </c>
-      <c r="F59" s="29" t="s">
+      <c r="F82" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="G59" s="31"/>
-      <c r="H59" s="44"/>
-      <c r="I59" s="18" t="s">
+      <c r="G82" s="31"/>
+      <c r="H82" s="43"/>
+      <c r="I82" s="18" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="32" customFormat="1" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+    <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B60" s="30" t="s">
+      <c r="B83" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C60" s="35" t="s">
+      <c r="C83" s="35" t="s">
         <v>261</v>
       </c>
-      <c r="D60" s="29" t="s">
+      <c r="D83" s="29" t="s">
         <v>243</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E83" s="30" t="s">
         <v>262</v>
       </c>
-      <c r="F60" s="29" t="s">
+      <c r="F83" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="G60" s="31"/>
-      <c r="H60" s="44"/>
-      <c r="I60" s="19" t="s">
+      <c r="G83" s="31"/>
+      <c r="H83" s="43"/>
+      <c r="I83" s="19" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="32" customFormat="1" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+    <row r="84" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B84" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="C61" s="35" t="s">
+      <c r="C84" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D61" s="29" t="s">
+      <c r="D84" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E84" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="F61" s="29" t="s">
+      <c r="F84" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="G61" s="31"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="18" t="s">
+      <c r="G84" s="31"/>
+      <c r="H84" s="43"/>
+      <c r="I84" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="32" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+    <row r="85" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B85" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C62" s="35" t="s">
+      <c r="C85" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="D62" s="29" t="s">
+      <c r="D85" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E85" s="30" t="s">
         <v>268</v>
       </c>
-      <c r="F62" s="29" t="s">
+      <c r="F85" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="G62" s="31"/>
-      <c r="H62" s="44"/>
-      <c r="I62" s="18" t="s">
+      <c r="G85" s="31"/>
+      <c r="H85" s="43"/>
+      <c r="I85" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="32" customFormat="1" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+    <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B86" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="C63" s="35" t="s">
+      <c r="C86" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="D63" s="29" t="s">
+      <c r="D86" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="E86" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F86" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="G63" s="31"/>
-      <c r="H63" s="44"/>
-      <c r="I63" s="18" t="s">
+      <c r="G86" s="31"/>
+      <c r="H86" s="43"/>
+      <c r="I86" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="23"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="25"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="25"/>
-      <c r="G64" s="27"/>
-      <c r="H64" s="25"/>
-      <c r="I64" s="28"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="7"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="8"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="8"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="7"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="7"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="15"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="7"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="15"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="7"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="15"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="7"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="15"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="7"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="8"/>
-      <c r="E72" s="15"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="7"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="15"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="14"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="7"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="15"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="14"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="7"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="15"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="7"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H77" s="8"/>
-      <c r="I77" s="7"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H78" s="8"/>
-      <c r="I78" s="7"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H79" s="8"/>
-      <c r="I79" s="7"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H80" s="8"/>
-      <c r="I80" s="7"/>
-    </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H81" s="8"/>
-      <c r="I81" s="7"/>
-    </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H82" s="8"/>
-      <c r="I82" s="7"/>
-    </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H83" s="8"/>
-      <c r="I83" s="7"/>
-    </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H84" s="8"/>
-      <c r="I84" s="7"/>
-    </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H85" s="8"/>
-      <c r="I85" s="7"/>
-    </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H86" s="8"/>
-      <c r="I86" s="7"/>
-    </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H87" s="8"/>
-      <c r="I87" s="7"/>
-    </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="23"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="25"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="25"/>
+      <c r="I87" s="28"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="8"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="14"/>
       <c r="H88" s="8"/>
       <c r="I88" s="7"/>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="8"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="14"/>
       <c r="H89" s="8"/>
       <c r="I89" s="7"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="8"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="14"/>
       <c r="H90" s="8"/>
       <c r="I90" s="7"/>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="8"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="14"/>
       <c r="H91" s="8"/>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="8"/>
+      <c r="G92" s="14"/>
       <c r="H92" s="8"/>
       <c r="I92" s="7"/>
     </row>
-    <row r="93" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H93" s="2"/>
-    </row>
-    <row r="94" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H101" s="2"/>
-    </row>
-    <row r="102" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H108" s="2"/>
-    </row>
-    <row r="109" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H109" s="2"/>
-    </row>
-    <row r="110" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H114" s="2"/>
-    </row>
-    <row r="115" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="7"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="7"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="7"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="8"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="7"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="8"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="8"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="7"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="8"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="7"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="8"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="7"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H100" s="8"/>
+      <c r="I100" s="7"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H101" s="8"/>
+      <c r="I101" s="7"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H102" s="8"/>
+      <c r="I102" s="7"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H103" s="8"/>
+      <c r="I103" s="7"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H104" s="8"/>
+      <c r="I104" s="7"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H105" s="8"/>
+      <c r="I105" s="7"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H106" s="8"/>
+      <c r="I106" s="7"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H107" s="8"/>
+      <c r="I107" s="7"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H108" s="8"/>
+      <c r="I108" s="7"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H109" s="8"/>
+      <c r="I109" s="7"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H110" s="8"/>
+      <c r="I110" s="7"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H111" s="8"/>
+      <c r="I111" s="7"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H112" s="8"/>
+      <c r="I112" s="7"/>
+    </row>
+    <row r="113" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H113" s="8"/>
+      <c r="I113" s="7"/>
+    </row>
+    <row r="114" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H114" s="8"/>
+      <c r="I114" s="7"/>
+    </row>
+    <row r="115" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H115" s="8"/>
+      <c r="I115" s="7"/>
+    </row>
+    <row r="116" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H116" s="2"/>
     </row>
-    <row r="117" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H117" s="2"/>
     </row>
-    <row r="118" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H118" s="2"/>
     </row>
-    <row r="119" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H119" s="2"/>
     </row>
-    <row r="120" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H120" s="2"/>
     </row>
-    <row r="121" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H121" s="2"/>
     </row>
-    <row r="122" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H122" s="2"/>
     </row>
-    <row r="123" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H123" s="2"/>
     </row>
-    <row r="124" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H124" s="2"/>
     </row>
-    <row r="125" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H125" s="2"/>
     </row>
-    <row r="126" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H126" s="2"/>
     </row>
-    <row r="127" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H127" s="2"/>
     </row>
-    <row r="128" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="8:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H128" s="2"/>
     </row>
     <row r="129" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -6193,19 +7103,88 @@
     <row r="964" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="H964" s="2"/>
     </row>
-    <row r="965" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="965" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H965" s="2"/>
     </row>
-    <row r="966" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="966" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H966" s="2"/>
     </row>
-    <row r="967" spans="8:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="967" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H967" s="2"/>
+    </row>
+    <row r="968" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H968" s="2"/>
+    </row>
+    <row r="969" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H969" s="2"/>
+    </row>
+    <row r="970" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H970" s="2"/>
+    </row>
+    <row r="971" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H971" s="2"/>
+    </row>
+    <row r="972" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H972" s="2"/>
+    </row>
+    <row r="973" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H973" s="2"/>
+    </row>
+    <row r="974" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H974" s="2"/>
+    </row>
+    <row r="975" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H975" s="2"/>
+    </row>
+    <row r="976" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H976" s="2"/>
+    </row>
+    <row r="977" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H977" s="2"/>
+    </row>
+    <row r="978" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H978" s="2"/>
+    </row>
+    <row r="979" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H979" s="2"/>
+    </row>
+    <row r="980" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H980" s="2"/>
+    </row>
+    <row r="981" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H981" s="2"/>
+    </row>
+    <row r="982" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H982" s="2"/>
+    </row>
+    <row r="983" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H983" s="2"/>
+    </row>
+    <row r="984" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H984" s="2"/>
+    </row>
+    <row r="985" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H985" s="2"/>
+    </row>
+    <row r="986" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H986" s="2"/>
+    </row>
+    <row r="987" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H987" s="2"/>
+    </row>
+    <row r="988" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H988" s="2"/>
+    </row>
+    <row r="989" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H989" s="2"/>
+    </row>
+    <row r="990" spans="8:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H990" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H967" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H31 H66:H990 H33:H65" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Status,Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6227,48 +7206,53 @@
     <hyperlink ref="I16" r:id="rId15" xr:uid="{56DB907C-E7E5-409C-BAC4-B63093F59AE0}"/>
     <hyperlink ref="I17" r:id="rId16" xr:uid="{C4AAC494-CB04-42CA-B143-F47C5A136347}"/>
     <hyperlink ref="I18" r:id="rId17" xr:uid="{635F8D8E-C364-4697-BED4-4CD432B2E1E2}"/>
-    <hyperlink ref="I27" r:id="rId18" xr:uid="{73669949-1CC1-4E59-9635-797EC53E2558}"/>
-    <hyperlink ref="I35" r:id="rId19" xr:uid="{C9A9E4FE-0F22-48A1-BAD8-B8E899FEE937}"/>
-    <hyperlink ref="I36" r:id="rId20" xr:uid="{F17BB888-4B79-4AE7-A1CA-DD939FBDCBAF}"/>
-    <hyperlink ref="I37" r:id="rId21" xr:uid="{7FAE4026-5664-414E-9F85-D59B777B25C6}"/>
-    <hyperlink ref="I38" r:id="rId22" xr:uid="{459BACFE-F7B9-41DF-A0F5-CE5467B714FE}"/>
-    <hyperlink ref="I39" r:id="rId23" xr:uid="{88D627F3-F074-4366-B25B-A11A24583671}"/>
-    <hyperlink ref="I40" r:id="rId24" xr:uid="{74E08284-750B-47E5-A389-D8FFB5C0B629}"/>
-    <hyperlink ref="I41" r:id="rId25" xr:uid="{DACA07E2-4503-4F74-8653-37F3658F51BD}"/>
-    <hyperlink ref="I42" r:id="rId26" xr:uid="{59D24FC6-2457-42DE-AD3E-DFFAF7537CF4}"/>
-    <hyperlink ref="I44" r:id="rId27" xr:uid="{062EAC22-6499-49DF-BBFD-1207C5141F99}"/>
-    <hyperlink ref="I45" r:id="rId28" xr:uid="{A98FF740-CE5B-4895-BB85-FB6C504CFDD3}"/>
-    <hyperlink ref="I60" r:id="rId29" xr:uid="{A06AC91B-A036-48B8-963D-787CE08A4FE4}"/>
-    <hyperlink ref="I53" r:id="rId30" xr:uid="{DCBDDD1D-1EBF-430C-ACB8-5DD4ADEADB0E}"/>
-    <hyperlink ref="I59" r:id="rId31" xr:uid="{14FA71FF-05BF-4AD9-87CA-9EC941E7293A}"/>
-    <hyperlink ref="I63" r:id="rId32" xr:uid="{C74D3AD0-E58F-4F84-AD11-8BD8A310F327}"/>
-    <hyperlink ref="I20" r:id="rId33" display="WireFrame_Client_001" xr:uid="{552F2AD0-97C0-4D8B-8D48-D4D7D7D25AB1}"/>
-    <hyperlink ref="I21" r:id="rId34" xr:uid="{23DD3708-BE9F-4BA0-9C5F-44FF7ED68297}"/>
-    <hyperlink ref="I22" r:id="rId35" xr:uid="{9A970034-423B-4957-81C9-2D894C098072}"/>
-    <hyperlink ref="I23" r:id="rId36" xr:uid="{E3DBBBAE-27ED-4992-906A-45F502066C5C}"/>
-    <hyperlink ref="I24" r:id="rId37" xr:uid="{05028FA7-4AC7-405F-90D0-8141152772C1}"/>
-    <hyperlink ref="I25" r:id="rId38" xr:uid="{EA86781D-68FB-4415-ADF0-0FDFB2F3E06C}"/>
-    <hyperlink ref="I26" r:id="rId39" xr:uid="{8E314A11-C5EE-4A2A-9D36-945873B2C541}"/>
-    <hyperlink ref="I28" r:id="rId40" xr:uid="{DEF7C337-EA2C-4914-A9A9-3792F3587454}"/>
-    <hyperlink ref="I29" r:id="rId41" xr:uid="{FA0EFD1B-9EEC-43EB-8B51-0A25F055346D}"/>
-    <hyperlink ref="I30" r:id="rId42" xr:uid="{729AC57A-FC2F-4B25-81DC-1173205E7D5F}"/>
-    <hyperlink ref="I31" r:id="rId43" xr:uid="{FD599400-41B8-42C8-864B-BC0201546A3C}"/>
-    <hyperlink ref="I32" r:id="rId44" xr:uid="{6398320B-D862-4EFD-B75C-E5AF085B2727}"/>
-    <hyperlink ref="I33" r:id="rId45" xr:uid="{0EB192E8-8EED-4520-9507-649A18E2C31F}"/>
-    <hyperlink ref="I52" r:id="rId46" display="..\WireFrame\Client_Home_page\Wireframe_Client_002.jpg" xr:uid="{F3E8432E-653B-458B-A95E-BA585DF9B193}"/>
-    <hyperlink ref="I46" r:id="rId47" xr:uid="{551D3E43-D002-4686-9FDA-368019E553B8}"/>
-    <hyperlink ref="I47" r:id="rId48" xr:uid="{000739D6-6E48-4782-87B1-B8450552F4E6}"/>
-    <hyperlink ref="I48" r:id="rId49" xr:uid="{D526E49A-1815-4647-B87A-9E14EBB57396}"/>
-    <hyperlink ref="I49" r:id="rId50" xr:uid="{9CBB436B-523F-4192-9EE2-7691C0DA2F60}"/>
-    <hyperlink ref="I50" r:id="rId51" xr:uid="{27AE55A4-941D-4CA9-A67D-C9FB0113A1B9}"/>
-    <hyperlink ref="I51" r:id="rId52" xr:uid="{0FF31057-A279-4D10-98A0-6E1FFFE2BBB1}"/>
-    <hyperlink ref="I54" r:id="rId53" xr:uid="{403DD631-8323-4A41-A768-8E3513232E6B}"/>
-    <hyperlink ref="I55" r:id="rId54" xr:uid="{0FA69A34-A2EB-4FD0-A486-07134BFDF1B8}"/>
-    <hyperlink ref="I56" r:id="rId55" xr:uid="{1E72292C-CBAE-4540-A382-D3B44AB8381A}"/>
-    <hyperlink ref="I62" r:id="rId56" xr:uid="{E749628A-FAF1-4532-88C9-1CDC50EE93DA}"/>
-    <hyperlink ref="I57" r:id="rId57" xr:uid="{1F7D4386-B865-4769-801C-C7B5A2E42A45}"/>
-    <hyperlink ref="I58" r:id="rId58" xr:uid="{F5BE3AFA-A38D-414C-9460-2CA943A253CB}"/>
-    <hyperlink ref="I61" r:id="rId59" xr:uid="{CD6CCB8D-07F0-461C-91CE-C84C1D40344E}"/>
+    <hyperlink ref="I40" r:id="rId18" xr:uid="{73669949-1CC1-4E59-9635-797EC53E2558}"/>
+    <hyperlink ref="I48" r:id="rId19" xr:uid="{C9A9E4FE-0F22-48A1-BAD8-B8E899FEE937}"/>
+    <hyperlink ref="I49" r:id="rId20" xr:uid="{F17BB888-4B79-4AE7-A1CA-DD939FBDCBAF}"/>
+    <hyperlink ref="I50" r:id="rId21" xr:uid="{7FAE4026-5664-414E-9F85-D59B777B25C6}"/>
+    <hyperlink ref="I51" r:id="rId22" xr:uid="{459BACFE-F7B9-41DF-A0F5-CE5467B714FE}"/>
+    <hyperlink ref="I52" r:id="rId23" xr:uid="{88D627F3-F074-4366-B25B-A11A24583671}"/>
+    <hyperlink ref="I53" r:id="rId24" xr:uid="{74E08284-750B-47E5-A389-D8FFB5C0B629}"/>
+    <hyperlink ref="I54" r:id="rId25" xr:uid="{DACA07E2-4503-4F74-8653-37F3658F51BD}"/>
+    <hyperlink ref="I55" r:id="rId26" xr:uid="{59D24FC6-2457-42DE-AD3E-DFFAF7537CF4}"/>
+    <hyperlink ref="I67" r:id="rId27" xr:uid="{062EAC22-6499-49DF-BBFD-1207C5141F99}"/>
+    <hyperlink ref="I68" r:id="rId28" xr:uid="{A98FF740-CE5B-4895-BB85-FB6C504CFDD3}"/>
+    <hyperlink ref="I83" r:id="rId29" xr:uid="{A06AC91B-A036-48B8-963D-787CE08A4FE4}"/>
+    <hyperlink ref="I76" r:id="rId30" xr:uid="{DCBDDD1D-1EBF-430C-ACB8-5DD4ADEADB0E}"/>
+    <hyperlink ref="I82" r:id="rId31" xr:uid="{14FA71FF-05BF-4AD9-87CA-9EC941E7293A}"/>
+    <hyperlink ref="I86" r:id="rId32" xr:uid="{C74D3AD0-E58F-4F84-AD11-8BD8A310F327}"/>
+    <hyperlink ref="I33" r:id="rId33" display="WireFrame_Client_001" xr:uid="{552F2AD0-97C0-4D8B-8D48-D4D7D7D25AB1}"/>
+    <hyperlink ref="I34" r:id="rId34" xr:uid="{23DD3708-BE9F-4BA0-9C5F-44FF7ED68297}"/>
+    <hyperlink ref="I35" r:id="rId35" xr:uid="{9A970034-423B-4957-81C9-2D894C098072}"/>
+    <hyperlink ref="I36" r:id="rId36" xr:uid="{E3DBBBAE-27ED-4992-906A-45F502066C5C}"/>
+    <hyperlink ref="I37" r:id="rId37" xr:uid="{05028FA7-4AC7-405F-90D0-8141152772C1}"/>
+    <hyperlink ref="I38" r:id="rId38" xr:uid="{EA86781D-68FB-4415-ADF0-0FDFB2F3E06C}"/>
+    <hyperlink ref="I39" r:id="rId39" xr:uid="{8E314A11-C5EE-4A2A-9D36-945873B2C541}"/>
+    <hyperlink ref="I41" r:id="rId40" xr:uid="{DEF7C337-EA2C-4914-A9A9-3792F3587454}"/>
+    <hyperlink ref="I42" r:id="rId41" xr:uid="{FA0EFD1B-9EEC-43EB-8B51-0A25F055346D}"/>
+    <hyperlink ref="I43" r:id="rId42" xr:uid="{729AC57A-FC2F-4B25-81DC-1173205E7D5F}"/>
+    <hyperlink ref="I44" r:id="rId43" xr:uid="{FD599400-41B8-42C8-864B-BC0201546A3C}"/>
+    <hyperlink ref="I45" r:id="rId44" xr:uid="{6398320B-D862-4EFD-B75C-E5AF085B2727}"/>
+    <hyperlink ref="I46" r:id="rId45" xr:uid="{0EB192E8-8EED-4520-9507-649A18E2C31F}"/>
+    <hyperlink ref="I75" r:id="rId46" display="..\WireFrame\Client_Home_page\Wireframe_Client_002.jpg" xr:uid="{F3E8432E-653B-458B-A95E-BA585DF9B193}"/>
+    <hyperlink ref="I69" r:id="rId47" xr:uid="{551D3E43-D002-4686-9FDA-368019E553B8}"/>
+    <hyperlink ref="I70" r:id="rId48" xr:uid="{000739D6-6E48-4782-87B1-B8450552F4E6}"/>
+    <hyperlink ref="I71" r:id="rId49" xr:uid="{D526E49A-1815-4647-B87A-9E14EBB57396}"/>
+    <hyperlink ref="I72" r:id="rId50" xr:uid="{9CBB436B-523F-4192-9EE2-7691C0DA2F60}"/>
+    <hyperlink ref="I73" r:id="rId51" xr:uid="{27AE55A4-941D-4CA9-A67D-C9FB0113A1B9}"/>
+    <hyperlink ref="I74" r:id="rId52" xr:uid="{0FF31057-A279-4D10-98A0-6E1FFFE2BBB1}"/>
+    <hyperlink ref="I77" r:id="rId53" xr:uid="{403DD631-8323-4A41-A768-8E3513232E6B}"/>
+    <hyperlink ref="I78" r:id="rId54" xr:uid="{0FA69A34-A2EB-4FD0-A486-07134BFDF1B8}"/>
+    <hyperlink ref="I79" r:id="rId55" xr:uid="{1E72292C-CBAE-4540-A382-D3B44AB8381A}"/>
+    <hyperlink ref="I85" r:id="rId56" xr:uid="{E749628A-FAF1-4532-88C9-1CDC50EE93DA}"/>
+    <hyperlink ref="I80" r:id="rId57" xr:uid="{1F7D4386-B865-4769-801C-C7B5A2E42A45}"/>
+    <hyperlink ref="I81" r:id="rId58" xr:uid="{F5BE3AFA-A38D-414C-9460-2CA943A253CB}"/>
+    <hyperlink ref="I84" r:id="rId59" xr:uid="{CD6CCB8D-07F0-461C-91CE-C84C1D40344E}"/>
+    <hyperlink ref="I56" r:id="rId60" xr:uid="{094ECC0C-0B96-4AAE-82AF-928EB7FC24B3}"/>
+    <hyperlink ref="I57" r:id="rId61" xr:uid="{73E44EF6-B644-41F8-BA59-4AA913479CB2}"/>
+    <hyperlink ref="I58" r:id="rId62" xr:uid="{2375578C-5AF8-454A-80B7-2B8771A2D188}"/>
+    <hyperlink ref="I59:I63" r:id="rId63" display="https://share.balsamiq.com/c/gSAJhmDq1Ff3FhHi1LzTBS.jpg" xr:uid="{5C74D1C5-3793-4CDD-862B-CE1921951BB0}"/>
+    <hyperlink ref="I64:I65" r:id="rId64" display="https://share.balsamiq.com/c/gSAJhmDq1Ff3FhHi1LzTBS.jpg" xr:uid="{801529ED-3584-4D17-B334-676B9C585E72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Doc: Updated Test data for test cases
</commit_message>
<xml_diff>
--- a/Test/Test-cases.xlsx
+++ b/Test/Test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A8B25-1F6D-45CE-8D06-84A8560A80F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C4C161-0852-4898-AC84-DB2ECA309B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="414">
   <si>
     <t>Test case ID</t>
   </si>
@@ -1670,16 +1670,225 @@
   <si>
     <t xml:space="preserve">Error message: "Invalid Data"	</t>
   </si>
+  <si>
+    <t>Username: TestUser
+Email: test@example.com
+Password: Pass1234
+Confirm Password: Pass1234
+Address: 123 Main St
+Phone: +201234567890
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: User123
+Email: user123@example.com
+Password: Pass1234
+Confirm Password: Pass1234
+Address: 12 Alpha Street
+Phone: +201111223344
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: Test User
+Email: testuser@example.com
+Password: TestUser12
+Confirm Password: TestUser12
+Address: 22 NoSpace Road
+Phone: +201112223344
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: ExistingUser
+Email: newuser@example.com
+Password: UniquePass1
+Confirm Password: UniquePass1
+Address: 88 Unique Lane
+Phone: +201100011122
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: EmailTest
+Email: invalid-email
+Password: EmailTest1
+Confirm Password: EmailTest1
+Address: 50 Email Rd
+Phone: +201123456789
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: SecondUser
+Email: duplicate@test.com
+Password: Duplicate1
+Confirm Password: Duplicate1
+Address: 17 Duplicate Ave
+Phone: +201109876543
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: ShortPass
+Email: shortpass@example.com
+Password: Pass123
+Confirm Password: Pass123
+Address: 45 Short St
+Phone: +201101010101
+National ID: 12345678901234
+</t>
+  </si>
+  <si>
+    <t>Username: HiddenUser
+Email: hidden@example.com
+Password: HiddenPass1
+Confirm Password: HiddenPass1
+Address: 31 Hidden Blvd
+Phone: +201105432198
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: MismatchUser
+Email: mismatch@example.com
+Password: Pass1234
+Confirm Password: Pass1235
+Address: 98 Mismatch St
+Phone: +201144455566
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: AddressUser
+Email: address@example.com
+Password: Address12
+Confirm Password: Address12
+Address: Main@St#
+Phone: +201177788899
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: LongAddress
+Email: longaddress@example.com
+Password: LongAddress1
+Confirm Password: LongAddress1
+Address: AAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAA1
+Phone: +201123443211
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username: PhoneChar
+Email: phonechar@example.com
+Password: PhoneChar1
+Confirm Password: PhoneChar1
+Address: 20 Alpha Rd
+Phone: +20abc123
+National ID: 12345678901234
+</t>
+  </si>
+  <si>
+    <t>Username: WrongPrefix
+Email: wrongprefix@example.com
+Password: WrongPrefix1
+Confirm Password: WrongPrefix1
+Address: 10 Prefix St
+Phone: 01234567890
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: SamePhone
+Email: samephone@example.com
+Password: SamePhone1
+Confirm Password: SamePhone1
+Address: 66 Phone Blvd
+Phone: +201112223344
+National ID: 12345678901234</t>
+  </si>
+  <si>
+    <t>Username: AlphaID
+Email: alphaid@example.com
+Password: AlphaID1
+Confirm Password: AlphaID1
+Address: 14 ID Lane
+Phone: +201155566677
+National ID: 1234567890abc</t>
+  </si>
+  <si>
+    <t>Username: ShortID
+Email: shortid@example.com
+Password: ShortID1
+Confirm Password: ShortID1
+Address: 12 Short ID Ave
+Phone: +201198765432
+National ID: 1234567890123</t>
+  </si>
+  <si>
+    <t>Username: User123
+Email: invalid-email
+Password: 123
+Confirm Password: 123
+Address: Main@St#
+Phone: 01234567890
+National ID: 1234567890abc</t>
+  </si>
+  <si>
+    <t>Username: "TestUser"
+Password: "Pass1234"</t>
+  </si>
+  <si>
+    <t>Username: "TestUser"
+Password: "Pass12345678"</t>
+  </si>
+  <si>
+    <t>Username: "   TestUser"
+Password: "Pass1234"</t>
+  </si>
+  <si>
+    <t>Username: " "
+Password: "Pass1234"</t>
+  </si>
+  <si>
+    <t>Username: "  "
+Password: " "</t>
+  </si>
+  <si>
+    <t>Username: " TestUser"
+Password: " "</t>
+  </si>
+  <si>
+    <t>Username: "TestUser"
+Password: "Pass1235"</t>
+  </si>
+  <si>
+    <t>Username: "TestUser"
+Password: "Pass123"</t>
+  </si>
+  <si>
+    <t>Username: "   TestUser"
+Password: "Pass1234a"</t>
+  </si>
+  <si>
+    <t>Username: "TestUser"
+Password: "Pass12345"</t>
+  </si>
+  <si>
+    <t>Username: "   TestUser"
+Password: "Pass12345"</t>
+  </si>
+  <si>
+    <t>Upoad Image</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1964,140 +2173,142 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{E2698182-7779-4DC2-A323-1BD467FFACE1}"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{9ED9F81B-D45E-4C2C-901A-F74EAD0E0F0B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2315,8 +2526,8 @@
   </sheetPr>
   <dimension ref="A1:J990"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="62" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="62" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2372,10 +2583,12 @@
       <c r="C2" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="59" t="s">
+        <v>385</v>
+      </c>
       <c r="F2" s="39" t="s">
         <v>59</v>
       </c>
@@ -2395,10 +2608,12 @@
       <c r="C3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="39"/>
+      <c r="E3" s="59" t="s">
+        <v>386</v>
+      </c>
       <c r="F3" s="39" t="s">
         <v>159</v>
       </c>
@@ -2418,10 +2633,12 @@
       <c r="C4" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="39"/>
+      <c r="E4" s="59" t="s">
+        <v>387</v>
+      </c>
       <c r="F4" s="39" t="s">
         <v>159</v>
       </c>
@@ -2441,10 +2658,12 @@
       <c r="C5" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="59" t="s">
+        <v>388</v>
+      </c>
       <c r="F5" s="39" t="s">
         <v>159</v>
       </c>
@@ -2464,10 +2683,12 @@
       <c r="C6" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="59" t="s">
+        <v>389</v>
+      </c>
       <c r="F6" s="47" t="s">
         <v>112</v>
       </c>
@@ -2487,10 +2708,12 @@
       <c r="C7" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="59" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="39"/>
+      <c r="E7" s="59" t="s">
+        <v>390</v>
+      </c>
       <c r="F7" s="47" t="s">
         <v>77</v>
       </c>
@@ -2510,10 +2733,12 @@
       <c r="C8" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="E8" s="39"/>
+      <c r="E8" s="59" t="s">
+        <v>391</v>
+      </c>
       <c r="F8" s="39" t="s">
         <v>159</v>
       </c>
@@ -2533,10 +2758,12 @@
       <c r="C9" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="59" t="s">
+        <v>392</v>
+      </c>
       <c r="F9" s="47" t="s">
         <v>84</v>
       </c>
@@ -2556,10 +2783,12 @@
       <c r="C10" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="59" t="s">
+        <v>393</v>
+      </c>
       <c r="F10" s="39" t="s">
         <v>159</v>
       </c>
@@ -2579,10 +2808,12 @@
       <c r="C11" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="59" t="s">
+        <v>394</v>
+      </c>
       <c r="F11" s="39" t="s">
         <v>112</v>
       </c>
@@ -2602,10 +2833,12 @@
       <c r="C12" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="59" t="s">
+        <v>395</v>
+      </c>
       <c r="F12" s="39" t="s">
         <v>112</v>
       </c>
@@ -2625,10 +2858,12 @@
       <c r="C13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="59" t="s">
+        <v>396</v>
+      </c>
       <c r="F13" s="47" t="s">
         <v>112</v>
       </c>
@@ -2648,10 +2883,12 @@
       <c r="C14" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="E14" s="39"/>
+      <c r="E14" s="59" t="s">
+        <v>397</v>
+      </c>
       <c r="F14" s="47" t="s">
         <v>112</v>
       </c>
@@ -2671,10 +2908,12 @@
       <c r="C15" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="59" t="s">
+        <v>398</v>
+      </c>
       <c r="F15" s="47" t="s">
         <v>77</v>
       </c>
@@ -2694,10 +2933,12 @@
       <c r="C16" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="39" t="s">
+      <c r="D16" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="59" t="s">
+        <v>399</v>
+      </c>
       <c r="F16" s="47" t="s">
         <v>112</v>
       </c>
@@ -2717,10 +2958,12 @@
       <c r="C17" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="59" t="s">
+        <v>400</v>
+      </c>
       <c r="F17" s="47" t="s">
         <v>112</v>
       </c>
@@ -2740,16 +2983,18 @@
       <c r="C18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="52" t="s">
+      <c r="E18" s="59" t="s">
+        <v>401</v>
+      </c>
+      <c r="F18" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="53"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="55" t="s">
+      <c r="G18" s="52"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="54" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2763,10 +3008,10 @@
       <c r="C19" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="59" t="s">
         <v>289</v>
       </c>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="60" t="s">
         <v>290</v>
       </c>
       <c r="F19" s="47" t="s">
@@ -2776,27 +3021,27 @@
       <c r="H19" s="47"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" s="60" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="57" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>291</v>
       </c>
-      <c r="B20" s="56" t="s">
+      <c r="B20" s="55" t="s">
         <v>292</v>
       </c>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="55" t="s">
         <v>288</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="58" t="s">
         <v>293</v>
       </c>
       <c r="E20" s="58" t="s">
         <v>294</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="56" t="s">
         <v>112</v>
       </c>
       <c r="G20" s="31"/>
-      <c r="H20" s="59"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="18"/>
     </row>
     <row r="21" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2809,10 +3054,10 @@
       <c r="C21" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="59" t="s">
         <v>298</v>
       </c>
       <c r="F21" s="47" t="s">
@@ -2832,10 +3077,10 @@
       <c r="C22" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="59" t="s">
         <v>302</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="59" t="s">
         <v>303</v>
       </c>
       <c r="F22" s="47" t="s">
@@ -2855,10 +3100,10 @@
       <c r="C23" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="59" t="s">
         <v>306</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="59" t="s">
         <v>307</v>
       </c>
       <c r="F23" s="47" t="s">
@@ -2878,10 +3123,10 @@
       <c r="C24" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="59" t="s">
         <v>310</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="59" t="s">
         <v>311</v>
       </c>
       <c r="F24" s="47" t="s">
@@ -2901,10 +3146,10 @@
       <c r="C25" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="59" t="s">
         <v>314</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="59" t="s">
         <v>315</v>
       </c>
       <c r="F25" s="47" t="s">
@@ -2924,10 +3169,10 @@
       <c r="C26" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="D26" s="59" t="s">
         <v>318</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="59" t="s">
         <v>319</v>
       </c>
       <c r="F26" s="47" t="s">
@@ -2947,10 +3192,10 @@
       <c r="C27" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="59" t="s">
         <v>323</v>
       </c>
       <c r="F27" s="47" t="s">
@@ -2970,10 +3215,10 @@
       <c r="C28" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D28" s="13" t="s">
+      <c r="D28" s="59" t="s">
         <v>326</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="59" t="s">
         <v>327</v>
       </c>
       <c r="F28" s="47" t="s">
@@ -2993,10 +3238,10 @@
       <c r="C29" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="59" t="s">
         <v>330</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="59" t="s">
         <v>331</v>
       </c>
       <c r="F29" s="47" t="s">
@@ -3016,10 +3261,10 @@
       <c r="C30" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D30" s="13" t="s">
+      <c r="D30" s="59" t="s">
         <v>334</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="59" t="s">
         <v>335</v>
       </c>
       <c r="F30" s="47" t="s">
@@ -3039,10 +3284,10 @@
       <c r="C31" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="59" t="s">
         <v>338</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="59" t="s">
         <v>339</v>
       </c>
       <c r="F31" s="47" t="s">
@@ -3066,7 +3311,9 @@
       <c r="D33" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="39"/>
+      <c r="E33" s="39" t="s">
+        <v>403</v>
+      </c>
       <c r="F33" s="39" t="s">
         <v>26</v>
       </c>
@@ -3089,7 +3336,9 @@
       <c r="D34" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="39"/>
+      <c r="E34" s="39" t="s">
+        <v>411</v>
+      </c>
       <c r="F34" s="39" t="s">
         <v>21</v>
       </c>
@@ -3112,7 +3361,9 @@
       <c r="D35" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="39"/>
+      <c r="E35" s="39" t="s">
+        <v>404</v>
+      </c>
       <c r="F35" s="39" t="s">
         <v>21</v>
       </c>
@@ -3135,7 +3386,9 @@
       <c r="D36" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="39"/>
+      <c r="E36" s="59" t="s">
+        <v>412</v>
+      </c>
       <c r="F36" s="39" t="s">
         <v>21</v>
       </c>
@@ -3158,7 +3411,9 @@
       <c r="D37" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="39"/>
+      <c r="E37" s="59" t="s">
+        <v>405</v>
+      </c>
       <c r="F37" s="39" t="s">
         <v>22</v>
       </c>
@@ -3181,7 +3436,9 @@
       <c r="D38" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="59" t="s">
+        <v>407</v>
+      </c>
       <c r="F38" s="39" t="s">
         <v>23</v>
       </c>
@@ -3204,7 +3461,9 @@
       <c r="D39" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="39"/>
+      <c r="E39" s="59" t="s">
+        <v>406</v>
+      </c>
       <c r="F39" s="39" t="s">
         <v>24</v>
       </c>
@@ -3227,7 +3486,9 @@
       <c r="D40" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E40" s="39"/>
+      <c r="E40" s="59" t="s">
+        <v>402</v>
+      </c>
       <c r="F40" s="39" t="s">
         <v>25</v>
       </c>
@@ -3250,7 +3511,9 @@
       <c r="D41" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E41" s="39"/>
+      <c r="E41" s="59" t="s">
+        <v>409</v>
+      </c>
       <c r="F41" s="39" t="s">
         <v>21</v>
       </c>
@@ -3273,7 +3536,9 @@
       <c r="D42" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="39"/>
+      <c r="E42" s="59" t="s">
+        <v>404</v>
+      </c>
       <c r="F42" s="39" t="s">
         <v>21</v>
       </c>
@@ -3283,7 +3548,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="32" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="32" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>37</v>
       </c>
@@ -3296,7 +3561,9 @@
       <c r="D43" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="39"/>
+      <c r="E43" s="59" t="s">
+        <v>410</v>
+      </c>
       <c r="F43" s="39" t="s">
         <v>21</v>
       </c>
@@ -3319,7 +3586,9 @@
       <c r="D44" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="39"/>
+      <c r="E44" s="59" t="s">
+        <v>405</v>
+      </c>
       <c r="F44" s="39" t="s">
         <v>22</v>
       </c>
@@ -3343,7 +3612,9 @@
       <c r="D45" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="E45" s="39"/>
+      <c r="E45" s="59" t="s">
+        <v>407</v>
+      </c>
       <c r="F45" s="39" t="s">
         <v>23</v>
       </c>
@@ -3367,7 +3638,9 @@
       <c r="D46" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="E46" s="39"/>
+      <c r="E46" s="59" t="s">
+        <v>408</v>
+      </c>
       <c r="F46" s="39" t="s">
         <v>21</v>
       </c>
@@ -3453,7 +3726,9 @@
       <c r="D50" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="39"/>
+      <c r="E50" s="39" t="s">
+        <v>413</v>
+      </c>
       <c r="F50" s="39" t="s">
         <v>158</v>
       </c>
@@ -7182,9 +7457,9 @@
       <c r="H990" s="2"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H31 H66:H990 H33:H65" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H31 H33:H990" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Status,Passed,Failed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Doc: Updated login test cases
</commit_message>
<xml_diff>
--- a/Test/Test-cases.xlsx
+++ b/Test/Test-cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ITI\Online-Mobile-Store-WebSite\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B473C78B-7CC0-4964-8844-0C74FE38E5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A16D48-5B00-4A05-A47A-5200D1B8B7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1549,9 +1549,6 @@
     <t>"Please enter valid username or password"</t>
   </si>
   <si>
-    <t>TC_Login_014+EA46:I46</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -2060,6 +2057,9 @@
   <si>
     <t>National ID = 20102091400148
 All other fields valid</t>
+  </si>
+  <si>
+    <t>TC_Login_014</t>
   </si>
 </sst>
 </file>
@@ -2388,7 +2388,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2550,15 +2550,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2813,8 +2804,8 @@
   </sheetPr>
   <dimension ref="A1:J977"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2877,13 +2868,13 @@
         <v>305</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>153</v>
@@ -2912,7 +2903,7 @@
         <v>133</v>
       </c>
       <c r="H3" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>135</v>
@@ -2941,7 +2932,7 @@
         <v>133</v>
       </c>
       <c r="H4" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>147</v>
@@ -2970,7 +2961,7 @@
         <v>133</v>
       </c>
       <c r="H5" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>146</v>
@@ -2999,7 +2990,7 @@
         <v>104</v>
       </c>
       <c r="H6" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>145</v>
@@ -3025,10 +3016,10 @@
         <v>69</v>
       </c>
       <c r="G7" s="29" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H7" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>136</v>
@@ -3057,7 +3048,7 @@
         <v>133</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>144</v>
@@ -3086,7 +3077,7 @@
         <v>76</v>
       </c>
       <c r="H9" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>136</v>
@@ -3115,7 +3106,7 @@
         <v>133</v>
       </c>
       <c r="H10" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>143</v>
@@ -3144,7 +3135,7 @@
         <v>104</v>
       </c>
       <c r="H11" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>142</v>
@@ -3173,7 +3164,7 @@
         <v>104</v>
       </c>
       <c r="H12" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>141</v>
@@ -3202,7 +3193,7 @@
         <v>104</v>
       </c>
       <c r="H13" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I13" s="7" t="s">
         <v>140</v>
@@ -3231,7 +3222,7 @@
         <v>104</v>
       </c>
       <c r="H14" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>139</v>
@@ -3257,10 +3248,10 @@
         <v>69</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H15" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>136</v>
@@ -3289,7 +3280,7 @@
         <v>104</v>
       </c>
       <c r="H16" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>138</v>
@@ -3318,7 +3309,7 @@
         <v>104</v>
       </c>
       <c r="H17" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>137</v>
@@ -3347,7 +3338,7 @@
         <v>104</v>
       </c>
       <c r="H18" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I18" s="33" t="s">
         <v>137</v>
@@ -3376,7 +3367,7 @@
         <v>104</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I19" s="7"/>
     </row>
@@ -3403,7 +3394,7 @@
         <v>104</v>
       </c>
       <c r="H20" s="42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I20" s="12"/>
     </row>
@@ -3427,10 +3418,10 @@
         <v>254</v>
       </c>
       <c r="G21" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H21" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I21" s="7"/>
     </row>
@@ -3457,7 +3448,7 @@
         <v>104</v>
       </c>
       <c r="H22" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I22" s="7"/>
     </row>
@@ -3481,10 +3472,10 @@
         <v>254</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I23" s="7"/>
     </row>
@@ -3508,10 +3499,10 @@
         <v>254</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H24" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I24" s="7"/>
     </row>
@@ -3538,7 +3529,7 @@
         <v>254</v>
       </c>
       <c r="H25" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I25" s="7"/>
     </row>
@@ -3565,7 +3556,7 @@
         <v>254</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I26" s="7"/>
     </row>
@@ -3592,7 +3583,7 @@
         <v>254</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I27" s="7"/>
     </row>
@@ -3619,7 +3610,7 @@
         <v>104</v>
       </c>
       <c r="H28" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I28" s="7"/>
     </row>
@@ -3646,7 +3637,7 @@
         <v>104</v>
       </c>
       <c r="H29" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I29" s="7"/>
     </row>
@@ -3673,7 +3664,7 @@
         <v>104</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I30" s="7"/>
     </row>
@@ -3700,25 +3691,25 @@
         <v>104</v>
       </c>
       <c r="H31" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I31" s="7"/>
     </row>
     <row r="32" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>243</v>
       </c>
       <c r="D32" s="63" t="s">
+        <v>455</v>
+      </c>
+      <c r="E32" s="24" t="s">
         <v>456</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>457</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>104</v>
@@ -3727,79 +3718,79 @@
         <v>104</v>
       </c>
       <c r="H32" s="65" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I32" s="66"/>
     </row>
     <row r="33" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>243</v>
       </c>
       <c r="D33" s="63" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F33" s="63" t="s">
         <v>254</v>
       </c>
       <c r="G33" s="64" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H33" s="65" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I33" s="66"/>
     </row>
     <row r="34" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>243</v>
       </c>
       <c r="D34" s="63" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F34" s="63" t="s">
         <v>254</v>
       </c>
       <c r="G34" s="64" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H34" s="65" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I34" s="66"/>
     </row>
     <row r="35" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B35" s="9" t="s">
         <v>466</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>467</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>243</v>
       </c>
       <c r="D35" s="24" t="s">
+        <v>467</v>
+      </c>
+      <c r="E35" s="24" t="s">
         <v>468</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>469</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>254</v>
@@ -3808,25 +3799,25 @@
         <v>254</v>
       </c>
       <c r="H35" s="41" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="B36" s="9" t="s">
         <v>470</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>471</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="24" t="s">
+        <v>471</v>
+      </c>
+      <c r="E36" s="24" t="s">
         <v>472</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>473</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>104</v>
@@ -3835,7 +3826,7 @@
         <v>104</v>
       </c>
       <c r="H36" s="39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I36" s="7" t="s">
         <v>141</v>
@@ -3843,28 +3834,28 @@
     </row>
     <row r="37" spans="1:9" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B37" s="63" t="s">
         <v>474</v>
-      </c>
-      <c r="B37" s="67" t="s">
-        <v>475</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="24" t="s">
+        <v>475</v>
+      </c>
+      <c r="E37" s="63" t="s">
         <v>476</v>
       </c>
-      <c r="E37" s="67" t="s">
-        <v>477</v>
-      </c>
-      <c r="F37" s="67" t="s">
+      <c r="F37" s="63" t="s">
         <v>254</v>
       </c>
-      <c r="G37" s="68" t="s">
+      <c r="G37" s="64" t="s">
         <v>254</v>
       </c>
-      <c r="H37" s="69" t="s">
-        <v>336</v>
+      <c r="H37" s="65" t="s">
+        <v>335</v>
       </c>
       <c r="I37" s="66"/>
     </row>
@@ -3889,13 +3880,13 @@
         <v>323</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G39" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H39" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I39" s="8" t="s">
         <v>156</v>
@@ -3918,13 +3909,13 @@
         <v>331</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G40" s="29" t="s">
         <v>334</v>
       </c>
       <c r="H40" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I40" s="7" t="s">
         <v>157</v>
@@ -3947,13 +3938,13 @@
         <v>324</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G41" s="29" t="s">
         <v>334</v>
       </c>
       <c r="H41" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I41" s="7" t="s">
         <v>157</v>
@@ -3976,13 +3967,13 @@
         <v>332</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G42" s="29" t="s">
         <v>334</v>
       </c>
       <c r="H42" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I42" s="7" t="s">
         <v>157</v>
@@ -4005,13 +3996,13 @@
         <v>325</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G43" s="29" t="s">
         <v>333</v>
       </c>
       <c r="H43" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>158</v>
@@ -4034,13 +4025,13 @@
         <v>327</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G44" s="29" t="s">
         <v>333</v>
       </c>
       <c r="H44" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I44" s="7" t="s">
         <v>159</v>
@@ -4063,13 +4054,13 @@
         <v>326</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G45" s="29" t="s">
         <v>333</v>
       </c>
       <c r="H45" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I45" s="7" t="s">
         <v>160</v>
@@ -4092,13 +4083,13 @@
         <v>322</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G46" s="29" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H46" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I46" s="7" t="s">
         <v>154</v>
@@ -4121,13 +4112,13 @@
         <v>329</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G47" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H47" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I47" s="7" t="s">
         <v>157</v>
@@ -4150,13 +4141,13 @@
         <v>324</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G48" s="29" t="s">
         <v>334</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I48" s="7" t="s">
         <v>157</v>
@@ -4179,13 +4170,13 @@
         <v>330</v>
       </c>
       <c r="F49" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G49" s="29" t="s">
         <v>334</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I49" s="7" t="s">
         <v>157</v>
@@ -4208,13 +4199,13 @@
         <v>325</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G50" s="29" t="s">
         <v>333</v>
       </c>
       <c r="H50" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I50" s="7" t="s">
         <v>158</v>
@@ -4238,13 +4229,13 @@
         <v>327</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G51" s="29" t="s">
         <v>333</v>
       </c>
       <c r="H51" s="44" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I51" s="7" t="s">
         <v>159</v>
@@ -4253,7 +4244,7 @@
     </row>
     <row r="52" spans="1:10" s="20" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>335</v>
+        <v>477</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>34</v>
@@ -4268,13 +4259,13 @@
         <v>328</v>
       </c>
       <c r="F52" s="36" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G52" s="19" t="s">
         <v>334</v>
       </c>
       <c r="H52" s="50" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I52" s="12" t="s">
         <v>157</v>
@@ -4313,7 +4304,7 @@
       </c>
       <c r="G54" s="19"/>
       <c r="H54" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I54" s="12" t="s">
         <v>149</v>
@@ -4340,7 +4331,7 @@
       </c>
       <c r="G55" s="19"/>
       <c r="H55" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I55" s="12" t="s">
         <v>149</v>
@@ -4367,7 +4358,7 @@
       </c>
       <c r="G56" s="19"/>
       <c r="H56" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I56" s="12" t="s">
         <v>149</v>
@@ -4394,7 +4385,7 @@
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I57" s="12" t="s">
         <v>149</v>
@@ -4421,7 +4412,7 @@
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I58" s="12" t="s">
         <v>149</v>
@@ -4448,7 +4439,7 @@
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I59" s="12" t="s">
         <v>149</v>
@@ -4475,7 +4466,7 @@
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="46" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I60" s="12" t="s">
         <v>149</v>
@@ -4501,10 +4492,10 @@
         <v>239</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H61" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I61" s="12" t="s">
         <v>149</v>
@@ -4530,10 +4521,10 @@
         <v>206</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H62" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I62" s="13" t="s">
         <v>240</v>
@@ -4559,10 +4550,10 @@
         <v>210</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H63" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I63" s="13" t="s">
         <v>150</v>
@@ -4588,10 +4579,10 @@
         <v>212</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H64" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I64" s="13" t="s">
         <v>150</v>
@@ -4617,10 +4608,10 @@
         <v>214</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H65" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I65" s="13" t="s">
         <v>150</v>
@@ -4646,10 +4637,10 @@
         <v>215</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H66" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I66" s="13" t="s">
         <v>150</v>
@@ -4675,10 +4666,10 @@
         <v>218</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H67" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I67" s="13" t="s">
         <v>150</v>
@@ -4704,10 +4695,10 @@
         <v>222</v>
       </c>
       <c r="G68" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H68" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I68" s="13" t="s">
         <v>150</v>
@@ -4733,10 +4724,10 @@
         <v>225</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H69" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I69" s="12" t="s">
         <v>155</v>
@@ -4762,10 +4753,10 @@
         <v>228</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H70" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I70" s="13" t="s">
         <v>151</v>
@@ -4791,10 +4782,10 @@
         <v>230</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H71" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I71" s="12" t="s">
         <v>148</v>
@@ -4823,7 +4814,7 @@
         <v>234</v>
       </c>
       <c r="H72" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I72" s="12" t="s">
         <v>148</v>
@@ -4849,10 +4840,10 @@
         <v>238</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H73" s="46" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I73" s="12" t="s">
         <v>148</v>
@@ -4874,28 +4865,28 @@
         <v>106</v>
       </c>
       <c r="B75" s="51" t="s">
+        <v>359</v>
+      </c>
+      <c r="C75" s="51" t="s">
         <v>360</v>
       </c>
-      <c r="C75" s="51" t="s">
-        <v>361</v>
-      </c>
       <c r="D75" s="62" t="s">
+        <v>421</v>
+      </c>
+      <c r="E75" s="62" t="s">
         <v>422</v>
       </c>
-      <c r="E75" s="62" t="s">
+      <c r="F75" s="62" t="s">
+        <v>438</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="H75" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I75" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="F75" s="62" t="s">
-        <v>439</v>
-      </c>
-      <c r="G75" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="H75" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4903,28 +4894,28 @@
         <v>107</v>
       </c>
       <c r="B76" s="51" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C76" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D76" s="62" t="s">
         <v>361</v>
       </c>
-      <c r="D76" s="62" t="s">
+      <c r="E76" s="51" t="s">
         <v>362</v>
       </c>
-      <c r="E76" s="51" t="s">
+      <c r="F76" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="F76" s="62" t="s">
-        <v>364</v>
-      </c>
       <c r="G76" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H76" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
@@ -4932,28 +4923,28 @@
         <v>108</v>
       </c>
       <c r="B77" s="51" t="s">
+        <v>364</v>
+      </c>
+      <c r="C77" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D77" s="62" t="s">
         <v>365</v>
       </c>
-      <c r="C77" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D77" s="62" t="s">
+      <c r="E77" s="51" t="s">
         <v>366</v>
       </c>
-      <c r="E77" s="51" t="s">
-        <v>367</v>
-      </c>
       <c r="F77" s="62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H77" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
@@ -4961,28 +4952,28 @@
         <v>109</v>
       </c>
       <c r="B78" s="51" t="s">
+        <v>367</v>
+      </c>
+      <c r="C78" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D78" s="62" t="s">
         <v>368</v>
       </c>
-      <c r="C78" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D78" s="62" t="s">
-        <v>369</v>
-      </c>
       <c r="E78" s="51" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F78" s="62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H78" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I78" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4990,28 +4981,28 @@
         <v>110</v>
       </c>
       <c r="B79" s="51" t="s">
+        <v>369</v>
+      </c>
+      <c r="C79" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D79" s="62" t="s">
         <v>370</v>
       </c>
-      <c r="C79" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D79" s="62" t="s">
+      <c r="E79" s="51" t="s">
         <v>371</v>
       </c>
-      <c r="E79" s="51" t="s">
-        <v>372</v>
-      </c>
       <c r="F79" s="62" t="s">
+        <v>427</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="H79" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I79" s="5" t="s">
         <v>428</v>
-      </c>
-      <c r="G79" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="H79" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I79" s="5" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5019,28 +5010,28 @@
         <v>111</v>
       </c>
       <c r="B80" s="51" t="s">
+        <v>372</v>
+      </c>
+      <c r="C80" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D80" s="62" t="s">
         <v>373</v>
       </c>
-      <c r="C80" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D80" s="62" t="s">
+      <c r="E80" s="51" t="s">
         <v>374</v>
       </c>
-      <c r="E80" s="51" t="s">
-        <v>375</v>
-      </c>
       <c r="F80" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="H80" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I80" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="H80" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5048,28 +5039,28 @@
         <v>112</v>
       </c>
       <c r="B81" s="51" t="s">
+        <v>375</v>
+      </c>
+      <c r="C81" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D81" s="62" t="s">
         <v>376</v>
       </c>
-      <c r="C81" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D81" s="62" t="s">
+      <c r="E81" s="51" t="s">
         <v>377</v>
       </c>
-      <c r="E81" s="51" t="s">
-        <v>378</v>
-      </c>
       <c r="F81" s="62" t="s">
+        <v>429</v>
+      </c>
+      <c r="G81" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="H81" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I81" s="5" t="s">
         <v>430</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="H81" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I81" s="5" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5077,28 +5068,28 @@
         <v>113</v>
       </c>
       <c r="B82" s="51" t="s">
+        <v>378</v>
+      </c>
+      <c r="C82" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D82" s="62" t="s">
         <v>379</v>
       </c>
-      <c r="C82" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D82" s="62" t="s">
+      <c r="E82" s="51" t="s">
         <v>380</v>
       </c>
-      <c r="E82" s="51" t="s">
-        <v>381</v>
-      </c>
       <c r="F82" s="62" t="s">
+        <v>431</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="H82" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I82" s="5" t="s">
         <v>432</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="H82" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I82" s="5" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -5106,28 +5097,28 @@
         <v>295</v>
       </c>
       <c r="B83" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="C83" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D83" s="62" t="s">
         <v>382</v>
       </c>
-      <c r="C83" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D83" s="62" t="s">
+      <c r="E83" s="51" t="s">
         <v>383</v>
       </c>
-      <c r="E83" s="51" t="s">
-        <v>384</v>
-      </c>
       <c r="F83" s="62" t="s">
+        <v>433</v>
+      </c>
+      <c r="G83" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="H83" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I83" s="5" t="s">
         <v>434</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="H83" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I83" s="5" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
@@ -5135,28 +5126,28 @@
         <v>296</v>
       </c>
       <c r="B84" s="51" t="s">
+        <v>384</v>
+      </c>
+      <c r="C84" s="51" t="s">
         <v>385</v>
       </c>
-      <c r="C84" s="51" t="s">
-        <v>386</v>
-      </c>
       <c r="D84" s="62" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E84" s="62" t="s">
+        <v>435</v>
+      </c>
+      <c r="F84" s="62" t="s">
         <v>436</v>
       </c>
-      <c r="F84" s="62" t="s">
+      <c r="G84" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="H84" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I84" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="H84" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -5164,25 +5155,25 @@
         <v>297</v>
       </c>
       <c r="B85" s="51" t="s">
+        <v>386</v>
+      </c>
+      <c r="C85" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D85" s="62" t="s">
         <v>387</v>
       </c>
-      <c r="C85" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D85" s="62" t="s">
-        <v>388</v>
-      </c>
       <c r="E85" s="51" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F85" s="62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G85" s="62" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H85" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I85" s="5"/>
     </row>
@@ -5191,25 +5182,25 @@
         <v>298</v>
       </c>
       <c r="B86" s="51" t="s">
+        <v>388</v>
+      </c>
+      <c r="C86" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D86" s="62" t="s">
         <v>389</v>
       </c>
-      <c r="C86" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D86" s="62" t="s">
+      <c r="E86" s="51" t="s">
         <v>390</v>
       </c>
-      <c r="E86" s="51" t="s">
-        <v>391</v>
-      </c>
       <c r="F86" s="62" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G86" s="62" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H86" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I86" s="5"/>
     </row>
@@ -5218,25 +5209,25 @@
         <v>299</v>
       </c>
       <c r="B87" s="51" t="s">
+        <v>391</v>
+      </c>
+      <c r="C87" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D87" s="62" t="s">
         <v>392</v>
       </c>
-      <c r="C87" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D87" s="62" t="s">
-        <v>393</v>
-      </c>
       <c r="E87" s="51" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F87" s="62" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G87" s="62" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H87" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I87" s="5"/>
     </row>
@@ -5245,25 +5236,25 @@
         <v>300</v>
       </c>
       <c r="B88" s="51" t="s">
+        <v>393</v>
+      </c>
+      <c r="C88" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D88" s="62" t="s">
         <v>394</v>
       </c>
-      <c r="C88" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D88" s="62" t="s">
-        <v>395</v>
-      </c>
       <c r="E88" s="51" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F88" s="62" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="G88" s="62" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H88" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I88" s="5"/>
     </row>
@@ -5272,25 +5263,25 @@
         <v>301</v>
       </c>
       <c r="B89" s="51" t="s">
+        <v>395</v>
+      </c>
+      <c r="C89" s="51" t="s">
+        <v>385</v>
+      </c>
+      <c r="D89" s="62" t="s">
         <v>396</v>
       </c>
-      <c r="C89" s="51" t="s">
-        <v>386</v>
-      </c>
-      <c r="D89" s="62" t="s">
-        <v>397</v>
-      </c>
       <c r="E89" s="51" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F89" s="62" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G89" s="62" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H89" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I89" s="5"/>
     </row>
@@ -5299,25 +5290,25 @@
         <v>302</v>
       </c>
       <c r="B90" s="51" t="s">
+        <v>397</v>
+      </c>
+      <c r="C90" s="51" t="s">
         <v>398</v>
       </c>
-      <c r="C90" s="51" t="s">
+      <c r="D90" s="62" t="s">
         <v>399</v>
       </c>
-      <c r="D90" s="62" t="s">
-        <v>400</v>
-      </c>
       <c r="E90" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="F90" s="62" t="s">
         <v>440</v>
       </c>
-      <c r="F90" s="62" t="s">
+      <c r="G90" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>442</v>
-      </c>
       <c r="H90" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I90" s="5"/>
     </row>
@@ -5326,28 +5317,28 @@
         <v>303</v>
       </c>
       <c r="B91" s="51" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C91" s="51" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D91" s="62" t="s">
+        <v>443</v>
+      </c>
+      <c r="E91" s="51" t="s">
         <v>444</v>
       </c>
-      <c r="E91" s="51" t="s">
+      <c r="F91" s="62" t="s">
         <v>445</v>
       </c>
-      <c r="F91" s="62" t="s">
+      <c r="G91" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="H91" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="I91" s="5" t="s">
         <v>446</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="H91" s="47" t="s">
-        <v>336</v>
-      </c>
-      <c r="I91" s="5" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.2">
@@ -5355,133 +5346,133 @@
         <v>304</v>
       </c>
       <c r="B92" s="51" t="s">
+        <v>401</v>
+      </c>
+      <c r="C92" s="51" t="s">
         <v>402</v>
       </c>
-      <c r="C92" s="51" t="s">
+      <c r="D92" s="62" t="s">
         <v>403</v>
       </c>
-      <c r="D92" s="62" t="s">
+      <c r="E92" s="51" t="s">
         <v>404</v>
       </c>
-      <c r="E92" s="51" t="s">
-        <v>405</v>
-      </c>
       <c r="F92" s="62" t="s">
+        <v>440</v>
+      </c>
+      <c r="G92" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="G92" s="3" t="s">
-        <v>442</v>
-      </c>
       <c r="H92" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I92" s="5"/>
     </row>
     <row r="93" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="51" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B93" s="51" t="s">
+        <v>405</v>
+      </c>
+      <c r="C93" s="51" t="s">
         <v>406</v>
       </c>
-      <c r="C93" s="51" t="s">
+      <c r="D93" s="62" t="s">
         <v>407</v>
       </c>
-      <c r="D93" s="62" t="s">
-        <v>408</v>
-      </c>
       <c r="E93" s="51" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F93" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G93" s="62" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H93" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I93" s="5"/>
     </row>
     <row r="94" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="51" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B94" s="51" t="s">
+        <v>408</v>
+      </c>
+      <c r="C94" s="51" t="s">
         <v>409</v>
       </c>
-      <c r="C94" s="51" t="s">
+      <c r="D94" s="62" t="s">
         <v>410</v>
       </c>
-      <c r="D94" s="62" t="s">
+      <c r="E94" s="51" t="s">
         <v>411</v>
       </c>
-      <c r="E94" s="51" t="s">
-        <v>412</v>
-      </c>
       <c r="F94" s="62" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="G94" s="62" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H94" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I94" s="5"/>
     </row>
     <row r="95" spans="1:9" ht="34.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="51" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B95" s="51" t="s">
+        <v>412</v>
+      </c>
+      <c r="C95" s="51" t="s">
         <v>413</v>
       </c>
-      <c r="C95" s="51" t="s">
+      <c r="D95" s="62" t="s">
         <v>414</v>
       </c>
-      <c r="D95" s="62" t="s">
+      <c r="E95" s="62" t="s">
         <v>415</v>
       </c>
-      <c r="E95" s="62" t="s">
+      <c r="F95" s="62" t="s">
         <v>416</v>
       </c>
-      <c r="F95" s="62" t="s">
-        <v>417</v>
-      </c>
       <c r="G95" s="62" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H95" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I95" s="5"/>
     </row>
     <row r="96" spans="1:9" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="51" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B96" s="51" t="s">
+        <v>448</v>
+      </c>
+      <c r="C96" s="51" t="s">
+        <v>360</v>
+      </c>
+      <c r="D96" s="62" t="s">
         <v>449</v>
       </c>
-      <c r="C96" s="51" t="s">
-        <v>361</v>
-      </c>
-      <c r="D96" s="62" t="s">
-        <v>450</v>
-      </c>
       <c r="E96" s="51" t="s">
+        <v>362</v>
+      </c>
+      <c r="F96" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="F96" s="62" t="s">
-        <v>364</v>
-      </c>
       <c r="G96" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H96" s="47" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I96" s="5"/>
     </row>

</xml_diff>